<commit_message>
everis suggestions for the mapping to eForms
</commit_message>
<xml_diff>
--- a/v2.0.1/Ontology_eForms_Mapping.xlsx
+++ b/v2.0.1/Ontology_eForms_Mapping.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\estaromi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jseguraf\Documents\GitHub\eprocurementontology\eprocurementontology\v2.0.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -407,7 +407,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12312" uniqueCount="1545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12335" uniqueCount="1562">
   <si>
     <t>ID</t>
   </si>
@@ -5954,9 +5954,6 @@
 (WG Approval 2019-01-22)</t>
   </si>
   <si>
-    <t>SubcontractTerms?</t>
-  </si>
-  <si>
     <r>
       <t>AwardCriterionEvaluationDimension.</t>
     </r>
@@ -7493,6 +7490,83 @@
   </si>
   <si>
     <t>Procedure.Lot.ContractTerms.ePayment.Indicator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SubcontractTerms?
+</t>
+  </si>
+  <si>
+    <t>Procedure has Lot,
+Lot has Contract Terms,
+Contract Terms has Subcontract Terms,
+Subontract Terms hasSubcontractRestriction Code</t>
+  </si>
+  <si>
+    <t>Procedure has Lot,
+Lot has Contract Terms,
+Contract Terms has Subcontract Terms,
+SubcontractTerms hasMinimumShare</t>
+  </si>
+  <si>
+    <t>Procedure has Lot,
+Lot has Contract Terms,
+Contract Terms has Subcontract Terms,
+Succontract Terms hasMaximumShare</t>
+  </si>
+  <si>
+    <t>Procedure has Lot,
+Award Criterion isUsedToAward Lot</t>
+  </si>
+  <si>
+    <t>Procedure has Lot,
+Award Criterion isUsedToAward Lot,
+Lot hasID Identifier</t>
+  </si>
+  <si>
+    <t>Procedure has Lot,
+Lot isReferredToIn Procurement Criterion Property,
+Procurement Criterion Property isa Property,
+Criterion has Information Criterion,
+Criterion has Award-Criterion-Property</t>
+  </si>
+  <si>
+    <t>Criterion hasName Text</t>
+  </si>
+  <si>
+    <t>Criterion hasDescription Text</t>
+  </si>
+  <si>
+    <t>AwardCriterion hasFixedValue Numeric</t>
+  </si>
+  <si>
+    <t>Criterion has weight-type</t>
+  </si>
+  <si>
+    <t>AwardCriterion has number-threshold</t>
+  </si>
+  <si>
+    <t>Procedure has Lot,
+Technique isUsedIn Lot</t>
+  </si>
+  <si>
+    <t>Procedure has Lot,
+Technique isUsedIn Lot,
+Lot hasID Identifier</t>
+  </si>
+  <si>
+    <t>Procedure uses Framework Agreement Terms,
+Framework Agreement Terms hasFrameworkAgreementType Code</t>
+  </si>
+  <si>
+    <t>Procedure uses Framework Agreement Terms,
+Framework Agreement Terms hasMaximumNumberofAwardedTenderers Amount</t>
+  </si>
+  <si>
+    <t>Procedure uses Framework Agreement Terms,
+Framework Agreement Terms hasDurationExtensionJustification Text</t>
+  </si>
+  <si>
+    <t>Everis mapping</t>
   </si>
 </sst>
 </file>
@@ -8742,7 +8816,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="286">
+  <cellXfs count="287">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -9444,6 +9518,12 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -9554,18 +9634,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="41">
+  <dxfs count="37">
     <dxf>
       <fill>
         <patternFill>
@@ -9584,34 +9661,6 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
         </patternFill>
       </fill>
     </dxf>
@@ -10026,7 +10075,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -10315,14 +10364,11 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:XFD300"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="B148" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BC2" sqref="BC2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" style="41" customWidth="1"/>
@@ -10360,95 +10406,99 @@
     <col min="50" max="50" width="33.140625" style="80" customWidth="1"/>
     <col min="51" max="51" width="45" style="80" customWidth="1"/>
     <col min="52" max="54" width="9.140625" style="58"/>
+    <col min="55" max="55" width="14.5703125" style="286" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:54" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="270" t="s">
+    <row r="1" spans="2:55" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="272" t="s">
         <v>205</v>
       </c>
-      <c r="C1" s="262" t="s">
+      <c r="C1" s="264" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="262" t="s">
+      <c r="D1" s="264" t="s">
         <v>577</v>
       </c>
-      <c r="E1" s="262" t="s">
+      <c r="E1" s="264" t="s">
         <v>319</v>
       </c>
-      <c r="F1" s="262" t="s">
+      <c r="F1" s="264" t="s">
         <v>330</v>
       </c>
-      <c r="G1" s="274" t="s">
+      <c r="G1" s="276" t="s">
         <v>333</v>
       </c>
-      <c r="H1" s="253" t="s">
+      <c r="H1" s="255" t="s">
         <v>540</v>
       </c>
-      <c r="I1" s="254"/>
-      <c r="J1" s="254"/>
-      <c r="K1" s="254"/>
-      <c r="L1" s="254"/>
-      <c r="M1" s="254"/>
-      <c r="N1" s="273"/>
-      <c r="O1" s="255"/>
-      <c r="P1" s="253" t="s">
+      <c r="I1" s="256"/>
+      <c r="J1" s="256"/>
+      <c r="K1" s="256"/>
+      <c r="L1" s="256"/>
+      <c r="M1" s="256"/>
+      <c r="N1" s="275"/>
+      <c r="O1" s="257"/>
+      <c r="P1" s="255" t="s">
         <v>541</v>
       </c>
-      <c r="Q1" s="254"/>
-      <c r="R1" s="254"/>
-      <c r="S1" s="254"/>
-      <c r="T1" s="254"/>
-      <c r="U1" s="254"/>
-      <c r="V1" s="254"/>
-      <c r="W1" s="254"/>
-      <c r="X1" s="254"/>
-      <c r="Y1" s="254"/>
-      <c r="Z1" s="254"/>
-      <c r="AA1" s="254"/>
-      <c r="AB1" s="254"/>
-      <c r="AC1" s="254"/>
-      <c r="AD1" s="255"/>
-      <c r="AE1" s="253" t="s">
+      <c r="Q1" s="256"/>
+      <c r="R1" s="256"/>
+      <c r="S1" s="256"/>
+      <c r="T1" s="256"/>
+      <c r="U1" s="256"/>
+      <c r="V1" s="256"/>
+      <c r="W1" s="256"/>
+      <c r="X1" s="256"/>
+      <c r="Y1" s="256"/>
+      <c r="Z1" s="256"/>
+      <c r="AA1" s="256"/>
+      <c r="AB1" s="256"/>
+      <c r="AC1" s="256"/>
+      <c r="AD1" s="257"/>
+      <c r="AE1" s="255" t="s">
         <v>542</v>
       </c>
-      <c r="AF1" s="254"/>
-      <c r="AG1" s="254"/>
-      <c r="AH1" s="255"/>
-      <c r="AI1" s="253" t="s">
+      <c r="AF1" s="256"/>
+      <c r="AG1" s="256"/>
+      <c r="AH1" s="257"/>
+      <c r="AI1" s="255" t="s">
         <v>543</v>
       </c>
-      <c r="AJ1" s="254"/>
-      <c r="AK1" s="254"/>
-      <c r="AL1" s="254"/>
-      <c r="AM1" s="254"/>
-      <c r="AN1" s="254"/>
-      <c r="AO1" s="254"/>
-      <c r="AP1" s="254"/>
-      <c r="AQ1" s="255"/>
-      <c r="AR1" s="253" t="s">
+      <c r="AJ1" s="256"/>
+      <c r="AK1" s="256"/>
+      <c r="AL1" s="256"/>
+      <c r="AM1" s="256"/>
+      <c r="AN1" s="256"/>
+      <c r="AO1" s="256"/>
+      <c r="AP1" s="256"/>
+      <c r="AQ1" s="257"/>
+      <c r="AR1" s="255" t="s">
         <v>963</v>
       </c>
-      <c r="AS1" s="254"/>
-      <c r="AT1" s="255"/>
-      <c r="AU1" s="258" t="s">
+      <c r="AS1" s="256"/>
+      <c r="AT1" s="257"/>
+      <c r="AU1" s="260" t="s">
         <v>1163</v>
       </c>
-      <c r="AV1" s="259" t="s">
+      <c r="AV1" s="261" t="s">
         <v>1149</v>
       </c>
-      <c r="AX1" s="260" t="s">
+      <c r="AX1" s="262" t="s">
         <v>971</v>
       </c>
-      <c r="AY1" s="261"/>
-      <c r="AZ1" s="261"/>
+      <c r="AY1" s="263"/>
+      <c r="AZ1" s="263"/>
+      <c r="BC1" s="286" t="s">
+        <v>1561</v>
+      </c>
     </row>
-    <row r="2" spans="2:54" ht="14.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="271"/>
-      <c r="C2" s="263"/>
-      <c r="D2" s="263"/>
-      <c r="E2" s="263"/>
-      <c r="F2" s="263"/>
-      <c r="G2" s="275"/>
+    <row r="2" spans="2:55" ht="14.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="273"/>
+      <c r="C2" s="265"/>
+      <c r="D2" s="265"/>
+      <c r="E2" s="265"/>
+      <c r="F2" s="265"/>
+      <c r="G2" s="277"/>
       <c r="H2" s="38">
         <v>1</v>
       </c>
@@ -10566,115 +10616,115 @@
       <c r="AT2" s="127">
         <v>39</v>
       </c>
-      <c r="AU2" s="258"/>
-      <c r="AV2" s="259"/>
+      <c r="AU2" s="260"/>
+      <c r="AV2" s="261"/>
       <c r="AW2" s="130"/>
-      <c r="AX2" s="248" t="s">
+      <c r="AX2" s="250" t="s">
         <v>972</v>
       </c>
-      <c r="AY2" s="248" t="s">
+      <c r="AY2" s="250" t="s">
         <v>973</v>
       </c>
-      <c r="AZ2" s="248" t="s">
+      <c r="AZ2" s="250" t="s">
         <v>974</v>
       </c>
       <c r="BA2" s="59"/>
-      <c r="BB2" s="248" t="s">
+      <c r="BB2" s="250" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="3" spans="2:54" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="271"/>
-      <c r="C3" s="263"/>
-      <c r="D3" s="263"/>
-      <c r="E3" s="263"/>
-      <c r="F3" s="263"/>
-      <c r="G3" s="275"/>
-      <c r="H3" s="266" t="s">
+    <row r="3" spans="2:55" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="273"/>
+      <c r="C3" s="265"/>
+      <c r="D3" s="265"/>
+      <c r="E3" s="265"/>
+      <c r="F3" s="265"/>
+      <c r="G3" s="277"/>
+      <c r="H3" s="268" t="s">
         <v>373</v>
       </c>
-      <c r="I3" s="257"/>
-      <c r="J3" s="269"/>
-      <c r="K3" s="268" t="s">
+      <c r="I3" s="259"/>
+      <c r="J3" s="271"/>
+      <c r="K3" s="270" t="s">
         <v>374</v>
       </c>
-      <c r="L3" s="257"/>
-      <c r="M3" s="269"/>
-      <c r="N3" s="268" t="s">
+      <c r="L3" s="259"/>
+      <c r="M3" s="271"/>
+      <c r="N3" s="270" t="s">
         <v>375</v>
       </c>
-      <c r="O3" s="265"/>
-      <c r="P3" s="266" t="s">
+      <c r="O3" s="267"/>
+      <c r="P3" s="268" t="s">
         <v>376</v>
       </c>
-      <c r="Q3" s="269"/>
-      <c r="R3" s="268" t="s">
+      <c r="Q3" s="271"/>
+      <c r="R3" s="270" t="s">
         <v>377</v>
       </c>
-      <c r="S3" s="257"/>
-      <c r="T3" s="269"/>
+      <c r="S3" s="259"/>
+      <c r="T3" s="271"/>
       <c r="U3" s="37" t="s">
         <v>562</v>
       </c>
-      <c r="V3" s="268" t="s">
+      <c r="V3" s="270" t="s">
         <v>378</v>
       </c>
-      <c r="W3" s="257"/>
-      <c r="X3" s="257"/>
-      <c r="Y3" s="269"/>
-      <c r="Z3" s="268" t="s">
+      <c r="W3" s="259"/>
+      <c r="X3" s="259"/>
+      <c r="Y3" s="271"/>
+      <c r="Z3" s="270" t="s">
         <v>379</v>
       </c>
-      <c r="AA3" s="269"/>
+      <c r="AA3" s="271"/>
       <c r="AB3" s="37" t="s">
         <v>680</v>
       </c>
-      <c r="AC3" s="268" t="s">
+      <c r="AC3" s="270" t="s">
         <v>681</v>
       </c>
-      <c r="AD3" s="265"/>
-      <c r="AE3" s="266" t="s">
+      <c r="AD3" s="267"/>
+      <c r="AE3" s="268" t="s">
         <v>682</v>
       </c>
-      <c r="AF3" s="257"/>
-      <c r="AG3" s="257"/>
-      <c r="AH3" s="265"/>
-      <c r="AI3" s="266" t="s">
+      <c r="AF3" s="259"/>
+      <c r="AG3" s="259"/>
+      <c r="AH3" s="267"/>
+      <c r="AI3" s="268" t="s">
         <v>382</v>
       </c>
-      <c r="AJ3" s="257"/>
-      <c r="AK3" s="257"/>
-      <c r="AL3" s="267"/>
-      <c r="AM3" s="256" t="s">
+      <c r="AJ3" s="259"/>
+      <c r="AK3" s="259"/>
+      <c r="AL3" s="269"/>
+      <c r="AM3" s="258" t="s">
         <v>383</v>
       </c>
-      <c r="AN3" s="257"/>
-      <c r="AO3" s="267"/>
-      <c r="AP3" s="256" t="s">
+      <c r="AN3" s="259"/>
+      <c r="AO3" s="269"/>
+      <c r="AP3" s="258" t="s">
         <v>681</v>
       </c>
-      <c r="AQ3" s="265"/>
-      <c r="AR3" s="256" t="s">
+      <c r="AQ3" s="267"/>
+      <c r="AR3" s="258" t="s">
         <v>963</v>
       </c>
-      <c r="AS3" s="257"/>
-      <c r="AT3" s="257"/>
-      <c r="AU3" s="258"/>
-      <c r="AV3" s="259"/>
+      <c r="AS3" s="259"/>
+      <c r="AT3" s="259"/>
+      <c r="AU3" s="260"/>
+      <c r="AV3" s="261"/>
       <c r="AW3" s="131"/>
-      <c r="AX3" s="249"/>
-      <c r="AY3" s="249"/>
-      <c r="AZ3" s="249"/>
+      <c r="AX3" s="251"/>
+      <c r="AY3" s="251"/>
+      <c r="AZ3" s="251"/>
       <c r="BA3" s="60"/>
-      <c r="BB3" s="249"/>
+      <c r="BB3" s="251"/>
     </row>
-    <row r="4" spans="2:54" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="272"/>
-      <c r="C4" s="264"/>
-      <c r="D4" s="264"/>
-      <c r="E4" s="264"/>
-      <c r="F4" s="264"/>
-      <c r="G4" s="276"/>
+    <row r="4" spans="2:55" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="274"/>
+      <c r="C4" s="266"/>
+      <c r="D4" s="266"/>
+      <c r="E4" s="266"/>
+      <c r="F4" s="266"/>
+      <c r="G4" s="278"/>
       <c r="H4" s="28" t="s">
         <v>386</v>
       </c>
@@ -10792,18 +10842,18 @@
       <c r="AT4" s="31" t="s">
         <v>389</v>
       </c>
-      <c r="AU4" s="258"/>
-      <c r="AV4" s="259"/>
+      <c r="AU4" s="260"/>
+      <c r="AV4" s="261"/>
       <c r="AW4" s="212" t="s">
-        <v>1317</v>
-      </c>
-      <c r="AX4" s="249"/>
-      <c r="AY4" s="249"/>
-      <c r="AZ4" s="249"/>
+        <v>1316</v>
+      </c>
+      <c r="AX4" s="251"/>
+      <c r="AY4" s="251"/>
+      <c r="AZ4" s="251"/>
       <c r="BA4" s="60"/>
-      <c r="BB4" s="249"/>
+      <c r="BB4" s="251"/>
     </row>
-    <row r="5" spans="2:54" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:55" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="201"/>
       <c r="C5" s="202"/>
       <c r="D5" s="202"/>
@@ -10851,16 +10901,16 @@
       <c r="AT5" s="208"/>
       <c r="AU5" s="204"/>
       <c r="AV5" s="213"/>
-      <c r="AW5" s="250" t="s">
-        <v>1314</v>
-      </c>
-      <c r="AX5" s="251"/>
-      <c r="AY5" s="252"/>
+      <c r="AW5" s="252" t="s">
+        <v>1313</v>
+      </c>
+      <c r="AX5" s="253"/>
+      <c r="AY5" s="254"/>
       <c r="AZ5" s="131"/>
       <c r="BA5" s="205"/>
       <c r="BB5" s="205"/>
     </row>
-    <row r="6" spans="2:54" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:55" ht="76.5" x14ac:dyDescent="0.2">
       <c r="B6" s="21" t="s">
         <v>206</v>
       </c>
@@ -11004,7 +11054,7 @@
       </c>
       <c r="AW6" s="214"/>
       <c r="AX6" s="215" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="AY6" s="215" t="s">
         <v>975</v>
@@ -11013,7 +11063,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="7" spans="2:54" ht="102" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:55" ht="102" x14ac:dyDescent="0.2">
       <c r="B7" s="106" t="s">
         <v>207</v>
       </c>
@@ -11151,7 +11201,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="8" spans="2:54" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:55" ht="127.5" x14ac:dyDescent="0.2">
       <c r="B8" s="106" t="s">
         <v>207</v>
       </c>
@@ -11292,10 +11342,10 @@
         <v>43662</v>
       </c>
       <c r="AW8" s="63" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="AX8" s="62" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="AY8" s="62" t="s">
         <v>979</v>
@@ -11307,7 +11357,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="9" spans="2:54" s="105" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:55" s="105" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B9" s="95" t="s">
         <v>207</v>
       </c>
@@ -11446,15 +11496,16 @@
       <c r="AU9" s="139"/>
       <c r="AV9" s="70"/>
       <c r="AW9" s="200" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="AX9" s="65"/>
       <c r="AY9" s="65"/>
       <c r="AZ9" s="66"/>
       <c r="BA9" s="66"/>
       <c r="BB9" s="67"/>
+      <c r="BC9" s="286"/>
     </row>
-    <row r="10" spans="2:54" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:55" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B10" s="181" t="s">
         <v>207</v>
       </c>
@@ -11597,7 +11648,7 @@
         <v>43662</v>
       </c>
       <c r="AW10" s="218" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="AX10" s="219" t="s">
         <v>981</v>
@@ -11611,7 +11662,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="11" spans="2:54" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:55" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B11" s="181" t="s">
         <v>207</v>
       </c>
@@ -11754,7 +11805,7 @@
         <v>43662</v>
       </c>
       <c r="AW11" s="218" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="AX11" s="219" t="s">
         <v>983</v>
@@ -11768,7 +11819,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="12" spans="2:54" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:55" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B12" s="181" t="s">
         <v>207</v>
       </c>
@@ -11909,7 +11960,7 @@
         <v>43662</v>
       </c>
       <c r="AW12" s="218" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="AX12" s="219" t="s">
         <v>985</v>
@@ -11923,7 +11974,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="13" spans="2:54" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:55" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B13" s="181" t="s">
         <v>207</v>
       </c>
@@ -12064,17 +12115,17 @@
         <v>43662</v>
       </c>
       <c r="AW13" s="218" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="AX13" s="219" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="AY13" s="145"/>
       <c r="AZ13" s="221"/>
       <c r="BA13" s="221"/>
       <c r="BB13" s="221"/>
     </row>
-    <row r="14" spans="2:54" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:55" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B14" s="181" t="s">
         <v>207</v>
       </c>
@@ -12215,17 +12266,17 @@
         <v>43662</v>
       </c>
       <c r="AW14" s="218" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="AX14" s="145" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="AY14" s="145"/>
       <c r="AZ14" s="221"/>
       <c r="BA14" s="221"/>
       <c r="BB14" s="221"/>
     </row>
-    <row r="15" spans="2:54" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:55" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B15" s="181" t="s">
         <v>207</v>
       </c>
@@ -12366,17 +12417,17 @@
         <v>43662</v>
       </c>
       <c r="AW15" s="218" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="AX15" s="145" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="AY15" s="145"/>
       <c r="AZ15" s="221"/>
       <c r="BA15" s="221"/>
       <c r="BB15" s="221"/>
     </row>
-    <row r="16" spans="2:54" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:55" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="181" t="s">
         <v>206</v>
       </c>
@@ -12512,7 +12563,7 @@
       </c>
       <c r="AW16" s="218"/>
       <c r="AX16" s="145" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="AY16" s="145"/>
       <c r="AZ16" s="145"/>
@@ -12654,16 +12705,16 @@
         <v>43662</v>
       </c>
       <c r="AW17" s="218" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="AX17" s="145" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="AY17" s="145"/>
       <c r="AZ17" s="145"/>
       <c r="BA17" s="145"/>
       <c r="BB17" s="145"/>
-      <c r="BC17"/>
+      <c r="BC17" s="286"/>
       <c r="BD17"/>
       <c r="BE17"/>
       <c r="BF17"/>
@@ -29129,10 +29180,10 @@
         <v>43662</v>
       </c>
       <c r="AW18" s="218" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="AX18" s="145" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="AY18" s="145"/>
       <c r="AZ18" s="145"/>
@@ -29275,7 +29326,7 @@
       </c>
       <c r="AW19" s="218"/>
       <c r="AX19" s="145" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="AY19" s="145"/>
       <c r="AZ19" s="145"/>
@@ -29583,6 +29634,7 @@
       <c r="AZ21" s="67"/>
       <c r="BA21" s="67"/>
       <c r="BB21" s="67"/>
+      <c r="BC21" s="286"/>
     </row>
     <row r="22" spans="2:16384" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B22" s="21" t="s">
@@ -29722,7 +29774,7 @@
       </c>
       <c r="AU22" s="139"/>
       <c r="AW22" s="91" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="AX22" s="72"/>
       <c r="AY22" s="72"/>
@@ -29868,7 +29920,7 @@
       </c>
       <c r="AU23" s="139"/>
       <c r="AW23" s="91" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="AX23" s="72"/>
       <c r="AY23" s="72"/>
@@ -30160,7 +30212,7 @@
       <c r="AU25" s="139"/>
       <c r="AW25" s="71"/>
       <c r="AX25" s="72" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="AY25" s="72"/>
       <c r="AZ25" s="73"/>
@@ -31189,7 +31241,7 @@
       <c r="BA32" s="73"/>
       <c r="BB32" s="73"/>
     </row>
-    <row r="33" spans="2:54" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:55" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="21" t="s">
         <v>207</v>
       </c>
@@ -31335,7 +31387,7 @@
       <c r="BA33" s="73"/>
       <c r="BB33" s="73"/>
     </row>
-    <row r="34" spans="2:54" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:55" x14ac:dyDescent="0.2">
       <c r="B34" s="21" t="s">
         <v>207</v>
       </c>
@@ -31481,7 +31533,7 @@
       <c r="BA34" s="73"/>
       <c r="BB34" s="73"/>
     </row>
-    <row r="35" spans="2:54" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:55" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B35" s="21" t="s">
         <v>207</v>
       </c>
@@ -31619,7 +31671,7 @@
       </c>
       <c r="AU35" s="139"/>
       <c r="AW35" s="91" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="AX35" s="72"/>
       <c r="AY35" s="72"/>
@@ -31627,7 +31679,7 @@
       <c r="BA35" s="73"/>
       <c r="BB35" s="73"/>
     </row>
-    <row r="36" spans="2:54" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:55" ht="114.75" x14ac:dyDescent="0.2">
       <c r="B36" s="181" t="s">
         <v>207</v>
       </c>
@@ -31765,17 +31817,17 @@
       </c>
       <c r="AU36" s="139"/>
       <c r="AW36" s="71" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="AX36" s="72" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="AY36" s="76"/>
       <c r="AZ36" s="77"/>
       <c r="BA36" s="77"/>
       <c r="BB36" s="77"/>
     </row>
-    <row r="37" spans="2:54" s="105" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:55" s="105" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="B37" s="95" t="s">
         <v>207</v>
       </c>
@@ -31923,8 +31975,9 @@
       <c r="BB37" s="66" t="s">
         <v>321</v>
       </c>
+      <c r="BC37" s="286"/>
     </row>
-    <row r="38" spans="2:54" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:55" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B38" s="21" t="s">
         <v>207</v>
       </c>
@@ -32060,7 +32113,7 @@
       </c>
       <c r="AW38" s="63"/>
       <c r="AX38" s="62" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="AY38" s="62" t="s">
         <v>996</v>
@@ -32073,7 +32126,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="39" spans="2:54" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:55" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B39" s="181" t="s">
         <v>208</v>
       </c>
@@ -32209,7 +32262,7 @@
       </c>
       <c r="AW39" s="63"/>
       <c r="AX39" s="62" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="AY39" s="62" t="s">
         <v>998</v>
@@ -32218,7 +32271,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="40" spans="2:54" s="197" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:55" s="197" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="B40" s="182" t="s">
         <v>208</v>
       </c>
@@ -32356,7 +32409,7 @@
       </c>
       <c r="AW40" s="218"/>
       <c r="AX40" s="193" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="AY40" s="194"/>
       <c r="AZ40" s="195"/>
@@ -32364,8 +32417,9 @@
       <c r="BB40" s="196" t="s">
         <v>321</v>
       </c>
+      <c r="BC40" s="286"/>
     </row>
-    <row r="41" spans="2:54" s="197" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:55" s="197" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B41" s="182" t="s">
         <v>208</v>
       </c>
@@ -32451,7 +32505,7 @@
       </c>
       <c r="AW41" s="218"/>
       <c r="AX41" s="193" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="AY41" s="194"/>
       <c r="AZ41" s="195"/>
@@ -32459,8 +32513,9 @@
       <c r="BB41" s="196" t="s">
         <v>328</v>
       </c>
+      <c r="BC41" s="286"/>
     </row>
-    <row r="42" spans="2:54" s="197" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:55" s="197" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B42" s="182" t="s">
         <v>208</v>
       </c>
@@ -32598,7 +32653,7 @@
       </c>
       <c r="AW42" s="218"/>
       <c r="AX42" s="193" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="AY42" s="194"/>
       <c r="AZ42" s="195"/>
@@ -32606,8 +32661,9 @@
       <c r="BB42" s="196" t="s">
         <v>321</v>
       </c>
+      <c r="BC42" s="286"/>
     </row>
-    <row r="43" spans="2:54" s="197" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:55" s="197" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B43" s="182" t="s">
         <v>208</v>
       </c>
@@ -32745,7 +32801,7 @@
       </c>
       <c r="AW43" s="218"/>
       <c r="AX43" s="193" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="AY43" s="194"/>
       <c r="AZ43" s="195"/>
@@ -32753,8 +32809,9 @@
       <c r="BB43" s="196" t="s">
         <v>321</v>
       </c>
+      <c r="BC43" s="286"/>
     </row>
-    <row r="44" spans="2:54" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:55" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B44" s="21" t="s">
         <v>207</v>
       </c>
@@ -32850,7 +32907,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="45" spans="2:54" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:55" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B45" s="21" t="s">
         <v>208</v>
       </c>
@@ -32995,7 +33052,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="46" spans="2:54" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:55" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="21" t="s">
         <v>208</v>
       </c>
@@ -33139,7 +33196,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="47" spans="2:54" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:55" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="21" t="s">
         <v>208</v>
       </c>
@@ -33236,7 +33293,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="48" spans="2:54" ht="102" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:55" ht="102" x14ac:dyDescent="0.2">
       <c r="B48" s="21" t="s">
         <v>206</v>
       </c>
@@ -33377,10 +33434,10 @@
         <v>43662</v>
       </c>
       <c r="AW48" s="218" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="AX48" s="62" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="AY48" s="62" t="s">
         <v>1006</v>
@@ -33531,7 +33588,7 @@
       </c>
       <c r="AW49" s="218"/>
       <c r="AX49" s="62" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
       <c r="AY49" s="62" t="s">
         <v>1007</v>
@@ -33681,7 +33738,7 @@
         <v>43664</v>
       </c>
       <c r="AW50" s="218" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="AX50" s="62"/>
       <c r="BB50" s="61"/>
@@ -33829,10 +33886,10 @@
         <v>43669</v>
       </c>
       <c r="AW51" s="218" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="AX51" s="62" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="AY51" s="78"/>
       <c r="BB51" s="58" t="s">
@@ -33982,7 +34039,7 @@
         <v>43669</v>
       </c>
       <c r="AW52" s="218" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="AX52" s="62" t="s">
         <v>1009</v>
@@ -34283,7 +34340,7 @@
       </c>
       <c r="AW54" s="218"/>
       <c r="AX54" s="62" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="AY54" s="70"/>
       <c r="BB54" s="61" t="s">
@@ -34431,10 +34488,10 @@
         <v>43669</v>
       </c>
       <c r="AW55" s="218" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="AX55" s="62" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="AY55" s="65" t="s">
         <v>1011</v>
@@ -34580,7 +34637,7 @@
         <v>43671</v>
       </c>
       <c r="AW56" s="218" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="57" spans="2:54" ht="63.75" x14ac:dyDescent="0.2">
@@ -34591,7 +34648,7 @@
         <v>36</v>
       </c>
       <c r="D57" s="42" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="E57" s="44" t="s">
         <v>320</v>
@@ -34720,10 +34777,10 @@
         <v>43671</v>
       </c>
       <c r="AW57" s="218" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="AX57" s="62" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="58" spans="2:54" ht="165.75" x14ac:dyDescent="0.2">
@@ -34863,10 +34920,10 @@
         <v>43671</v>
       </c>
       <c r="AW58" s="218" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="AX58" s="62" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="59" spans="2:54" ht="127.5" x14ac:dyDescent="0.2">
@@ -35009,10 +35066,10 @@
         <v>1153</v>
       </c>
       <c r="AV59" s="225" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="AW59" s="218" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="AX59" s="62"/>
       <c r="AY59" s="62" t="s">
@@ -35160,7 +35217,7 @@
         <v>43671</v>
       </c>
       <c r="AW60" s="218" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="AX60" s="62"/>
       <c r="AY60" s="62" t="s">
@@ -35310,13 +35367,13 @@
         <v>1180</v>
       </c>
       <c r="AV61" s="138" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="AW61" s="218" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="AX61" s="62" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="AY61" s="78"/>
     </row>
@@ -35460,13 +35517,13 @@
         <v>1179</v>
       </c>
       <c r="AV62" s="138" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="AW62" s="218" t="s">
+        <v>1346</v>
+      </c>
+      <c r="AX62" s="62" t="s">
         <v>1347</v>
-      </c>
-      <c r="AX62" s="62" t="s">
-        <v>1348</v>
       </c>
       <c r="AY62" s="78"/>
     </row>
@@ -35610,11 +35667,11 @@
         <v>1209</v>
       </c>
       <c r="AV63" s="167" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="AW63" s="218"/>
       <c r="AX63" s="62" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="64" spans="2:54" ht="76.5" x14ac:dyDescent="0.2">
@@ -35757,13 +35814,13 @@
         <v>1272</v>
       </c>
       <c r="AV64" s="167" t="s">
+        <v>1348</v>
+      </c>
+      <c r="AW64" s="218" t="s">
+        <v>1350</v>
+      </c>
+      <c r="AX64" s="62" t="s">
         <v>1349</v>
-      </c>
-      <c r="AW64" s="218" t="s">
-        <v>1351</v>
-      </c>
-      <c r="AX64" s="62" t="s">
-        <v>1350</v>
       </c>
       <c r="AY64" s="78"/>
     </row>
@@ -35907,13 +35964,13 @@
         <v>1209</v>
       </c>
       <c r="AV65" s="226" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="AW65" s="198" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="AX65" s="62" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="AY65" s="80" t="s">
         <v>1262</v>
@@ -36215,13 +36272,13 @@
         <v>1273</v>
       </c>
       <c r="AV67" s="227" t="s">
+        <v>1354</v>
+      </c>
+      <c r="AW67" s="229" t="s">
+        <v>1358</v>
+      </c>
+      <c r="AX67" s="62" t="s">
         <v>1355</v>
-      </c>
-      <c r="AW67" s="229" t="s">
-        <v>1359</v>
-      </c>
-      <c r="AX67" s="62" t="s">
-        <v>1356</v>
       </c>
       <c r="BB67" s="58" t="s">
         <v>328</v>
@@ -36367,13 +36424,13 @@
         <v>1212</v>
       </c>
       <c r="AV68" s="227" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="AW68" s="229" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="AX68" s="62" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="AY68" s="80" t="s">
         <v>1224</v>
@@ -36520,10 +36577,10 @@
       </c>
       <c r="AU69" s="139"/>
       <c r="AV69" s="154" t="s">
+        <v>1373</v>
+      </c>
+      <c r="AW69" s="229" t="s">
         <v>1374</v>
-      </c>
-      <c r="AW69" s="229" t="s">
-        <v>1375</v>
       </c>
       <c r="AX69" s="62"/>
       <c r="AY69" s="62"/>
@@ -36669,10 +36726,10 @@
         <v>43671</v>
       </c>
       <c r="AW70" s="229" t="s">
+        <v>1375</v>
+      </c>
+      <c r="AX70" s="63" t="s">
         <v>1376</v>
-      </c>
-      <c r="AX70" s="63" t="s">
-        <v>1377</v>
       </c>
       <c r="BB70" s="224" t="s">
         <v>320</v>
@@ -36819,10 +36876,10 @@
         <v>43671</v>
       </c>
       <c r="AW71" s="229" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
       <c r="AX71" s="62" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
       <c r="BB71" s="61" t="s">
         <v>324</v>
@@ -36969,10 +37026,10 @@
         <v>43671</v>
       </c>
       <c r="AW72" s="229" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
       <c r="AX72" s="62" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="BB72" s="61" t="s">
         <v>324</v>
@@ -37119,10 +37176,10 @@
         <v>43671</v>
       </c>
       <c r="AW73" s="229" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
       <c r="AX73" s="62" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
       <c r="BB73" s="61" t="s">
         <v>324</v>
@@ -37269,10 +37326,10 @@
         <v>43671</v>
       </c>
       <c r="AW74" s="229" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="AX74" s="62" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="75" spans="2:54" ht="63.75" x14ac:dyDescent="0.2">
@@ -37416,10 +37473,10 @@
         <v>43671</v>
       </c>
       <c r="AW75" s="229" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
       <c r="AX75" s="62" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="76" spans="2:54" ht="140.25" x14ac:dyDescent="0.2">
@@ -37562,16 +37619,16 @@
         <v>1209</v>
       </c>
       <c r="AV76" s="228" t="s">
+        <v>1364</v>
+      </c>
+      <c r="AW76" s="229" t="s">
+        <v>1366</v>
+      </c>
+      <c r="AX76" s="62" t="s">
         <v>1365</v>
       </c>
-      <c r="AW76" s="229" t="s">
-        <v>1367</v>
-      </c>
-      <c r="AX76" s="62" t="s">
-        <v>1366</v>
-      </c>
       <c r="AY76" s="62" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
       <c r="BB76" s="178" t="s">
         <v>321</v>
@@ -37717,13 +37774,13 @@
         <v>1268</v>
       </c>
       <c r="AV77" s="230" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="AW77" s="218" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="AX77" s="62" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="AY77" s="62" t="s">
         <v>1269</v>
@@ -37868,7 +37925,7 @@
       <c r="AU78" s="139"/>
       <c r="AW78" s="218"/>
       <c r="AX78" s="62" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="AY78" s="62"/>
       <c r="BB78" s="61" t="s">
@@ -38016,10 +38073,10 @@
       </c>
       <c r="AW79" s="231"/>
       <c r="AX79" s="62" t="s">
+        <v>1379</v>
+      </c>
+      <c r="AY79" s="62" t="s">
         <v>1380</v>
-      </c>
-      <c r="AY79" s="62" t="s">
-        <v>1381</v>
       </c>
     </row>
     <row r="80" spans="2:54" ht="51" x14ac:dyDescent="0.2">
@@ -38159,16 +38216,16 @@
         <v>371</v>
       </c>
       <c r="AU80" s="139" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="AV80" s="216">
         <v>43678</v>
       </c>
       <c r="AW80" s="218" t="s">
+        <v>1382</v>
+      </c>
+      <c r="AX80" s="62" t="s">
         <v>1383</v>
-      </c>
-      <c r="AX80" s="62" t="s">
-        <v>1384</v>
       </c>
       <c r="AY80" s="62" t="s">
         <v>1014</v>
@@ -38314,16 +38371,16 @@
         <v>371</v>
       </c>
       <c r="AU81" s="139" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="AV81" s="216">
         <v>43678</v>
       </c>
       <c r="AW81" s="218" t="s">
+        <v>1384</v>
+      </c>
+      <c r="AX81" s="62" t="s">
         <v>1385</v>
-      </c>
-      <c r="AX81" s="62" t="s">
-        <v>1386</v>
       </c>
       <c r="AY81" s="62" t="s">
         <v>1015</v>
@@ -38473,10 +38530,10 @@
         <v>43678</v>
       </c>
       <c r="AW82" s="218" t="s">
+        <v>1386</v>
+      </c>
+      <c r="AX82" s="62" t="s">
         <v>1387</v>
-      </c>
-      <c r="AX82" s="62" t="s">
-        <v>1388</v>
       </c>
       <c r="AY82" s="83" t="s">
         <v>1016</v>
@@ -38625,16 +38682,16 @@
         <v>1191</v>
       </c>
       <c r="AV83" s="235" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="AW83" s="218" t="s">
+        <v>1388</v>
+      </c>
+      <c r="AX83" s="62" t="s">
         <v>1389</v>
       </c>
-      <c r="AX83" s="62" t="s">
+      <c r="AY83" s="62" t="s">
         <v>1390</v>
-      </c>
-      <c r="AY83" s="62" t="s">
-        <v>1391</v>
       </c>
     </row>
     <row r="84" spans="2:54" ht="229.5" x14ac:dyDescent="0.25">
@@ -38774,19 +38831,19 @@
         <v>371</v>
       </c>
       <c r="AU84" s="151" t="s">
+        <v>1392</v>
+      </c>
+      <c r="AV84" s="230" t="s">
         <v>1393</v>
       </c>
-      <c r="AV84" s="230" t="s">
+      <c r="AW84" s="218" t="s">
         <v>1394</v>
       </c>
-      <c r="AW84" s="218" t="s">
+      <c r="AX84" s="62" t="s">
         <v>1395</v>
       </c>
-      <c r="AX84" s="62" t="s">
+      <c r="AY84" s="62" t="s">
         <v>1396</v>
-      </c>
-      <c r="AY84" s="62" t="s">
-        <v>1397</v>
       </c>
       <c r="BB84" s="178" t="s">
         <v>1025</v>
@@ -38932,13 +38989,13 @@
         <v>1209</v>
       </c>
       <c r="AV85" s="230" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="AW85" s="218" t="s">
+        <v>1397</v>
+      </c>
+      <c r="AX85" s="62" t="s">
         <v>1398</v>
-      </c>
-      <c r="AX85" s="62" t="s">
-        <v>1399</v>
       </c>
       <c r="BB85" s="61" t="s">
         <v>324</v>
@@ -39227,10 +39284,10 @@
         <v>43697</v>
       </c>
       <c r="AW87" s="236" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="AX87" s="80" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="88" spans="2:54" ht="216.75" x14ac:dyDescent="0.2">
@@ -39370,19 +39427,19 @@
         <v>371</v>
       </c>
       <c r="AU88" s="239" t="s">
+        <v>1445</v>
+      </c>
+      <c r="AV88" s="240" t="s">
         <v>1446</v>
       </c>
-      <c r="AV88" s="240" t="s">
-        <v>1447</v>
-      </c>
       <c r="AW88" s="236" t="s">
+        <v>1443</v>
+      </c>
+      <c r="AX88" s="62" t="s">
         <v>1444</v>
       </c>
-      <c r="AX88" s="62" t="s">
-        <v>1445</v>
-      </c>
       <c r="AY88" s="80" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="BB88" s="61" t="s">
         <v>328</v>
@@ -39525,7 +39582,7 @@
         <v>229</v>
       </c>
       <c r="AY89" s="179" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="BB89" s="61" t="s">
         <v>1020</v>
@@ -39662,16 +39719,16 @@
       <c r="AS90" s="23"/>
       <c r="AT90" s="24"/>
       <c r="AU90" s="139" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="AV90" s="216">
         <v>43697</v>
       </c>
       <c r="AW90" s="236" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
       <c r="AX90" s="80" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="AY90" s="84"/>
     </row>
@@ -39812,19 +39869,19 @@
         <v>43697</v>
       </c>
       <c r="AW91" s="236" t="s">
+        <v>1405</v>
+      </c>
+      <c r="AX91" s="62" t="s">
         <v>1406</v>
       </c>
-      <c r="AX91" s="62" t="s">
+      <c r="AY91" s="179" t="s">
         <v>1407</v>
-      </c>
-      <c r="AY91" s="179" t="s">
-        <v>1408</v>
       </c>
       <c r="BB91" s="58" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="92" spans="2:54" ht="153" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:54" ht="165.75" x14ac:dyDescent="0.2">
       <c r="B92" s="21" t="s">
         <v>207</v>
       </c>
@@ -39959,13 +40016,13 @@
         <v>43697</v>
       </c>
       <c r="AW92" s="216" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="AX92" s="62" t="s">
         <v>1021</v>
       </c>
       <c r="AY92" s="179" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
       <c r="BB92" s="58" t="s">
         <v>324</v>
@@ -40112,13 +40169,13 @@
         <v>43697</v>
       </c>
       <c r="AW93" s="145" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
       <c r="AX93" s="80" t="s">
         <v>1022</v>
       </c>
       <c r="AY93" s="80" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
       <c r="BB93" s="58" t="s">
         <v>328</v>
@@ -40199,7 +40256,7 @@
         <v>43697</v>
       </c>
       <c r="AW94" s="145" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="AX94" s="62" t="s">
         <v>1225</v>
@@ -40351,10 +40408,10 @@
         <v>1213</v>
       </c>
       <c r="AV95" s="237" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="AW95" s="218" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="AX95" s="62"/>
       <c r="AY95" s="62"/>
@@ -40500,10 +40557,10 @@
         <v>1194</v>
       </c>
       <c r="AV96" s="237" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="AW96" s="218" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="AX96" s="62"/>
       <c r="AY96" s="62"/>
@@ -40647,10 +40704,10 @@
         <v>1210</v>
       </c>
       <c r="AV97" s="237" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="AW97" s="218" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="AX97" s="62"/>
       <c r="AY97" s="62"/>
@@ -40799,7 +40856,7 @@
         <v>43697</v>
       </c>
       <c r="AW98" s="219" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
       <c r="AX98" s="62" t="s">
         <v>1023</v>
@@ -40906,13 +40963,13 @@
         <v>43697</v>
       </c>
       <c r="AW99" s="219" t="s">
+        <v>1417</v>
+      </c>
+      <c r="AX99" s="62" t="s">
         <v>1418</v>
       </c>
-      <c r="AX99" s="62" t="s">
+      <c r="AY99" s="62" t="s">
         <v>1419</v>
-      </c>
-      <c r="AY99" s="62" t="s">
-        <v>1420</v>
       </c>
       <c r="AZ99" s="234"/>
       <c r="BA99" s="234"/>
@@ -41061,10 +41118,10 @@
         <v>43699</v>
       </c>
       <c r="AW100" s="219" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="AX100" s="62" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="AY100" s="80" t="s">
         <v>727</v>
@@ -41355,10 +41412,10 @@
         <v>43699</v>
       </c>
       <c r="AW102" s="219" t="s">
+        <v>1422</v>
+      </c>
+      <c r="AX102" s="62" t="s">
         <v>1423</v>
-      </c>
-      <c r="AX102" s="62" t="s">
-        <v>1424</v>
       </c>
       <c r="AY102" s="62"/>
       <c r="BB102" s="61" t="s">
@@ -41506,10 +41563,10 @@
         <v>43699</v>
       </c>
       <c r="AW103" s="219" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="AX103" s="62" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="BB103" s="61" t="s">
         <v>320</v>
@@ -41658,10 +41715,10 @@
         <v>43699</v>
       </c>
       <c r="AW104" s="219" t="s">
+        <v>1427</v>
+      </c>
+      <c r="AX104" s="62" t="s">
         <v>1428</v>
-      </c>
-      <c r="AX104" s="62" t="s">
-        <v>1429</v>
       </c>
       <c r="AY104" s="62" t="s">
         <v>1026</v>
@@ -41811,10 +41868,10 @@
         <v>43699</v>
       </c>
       <c r="AW105" s="219" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="AX105" s="80" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="106" spans="2:54" ht="76.5" x14ac:dyDescent="0.2">
@@ -41958,10 +42015,10 @@
         <v>43699</v>
       </c>
       <c r="AW106" s="219" t="s">
+        <v>1430</v>
+      </c>
+      <c r="AX106" s="62" t="s">
         <v>1431</v>
-      </c>
-      <c r="AX106" s="62" t="s">
-        <v>1432</v>
       </c>
       <c r="AY106" s="62" t="s">
         <v>1027</v>
@@ -42111,10 +42168,10 @@
         <v>43699</v>
       </c>
       <c r="AW107" s="219" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
       <c r="AX107" s="62" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="AY107" s="62" t="s">
         <v>1028</v>
@@ -42266,13 +42323,13 @@
         <v>43699</v>
       </c>
       <c r="AW108" s="219" t="s">
+        <v>1435</v>
+      </c>
+      <c r="AX108" s="80" t="s">
+        <v>1434</v>
+      </c>
+      <c r="AY108" s="80" t="s">
         <v>1436</v>
-      </c>
-      <c r="AX108" s="80" t="s">
-        <v>1435</v>
-      </c>
-      <c r="AY108" s="80" t="s">
-        <v>1437</v>
       </c>
       <c r="BB108" s="58" t="s">
         <v>328</v>
@@ -42416,13 +42473,13 @@
       </c>
       <c r="AU109" s="159"/>
       <c r="AV109" s="167" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="AW109" s="219" t="s">
+        <v>1437</v>
+      </c>
+      <c r="AX109" s="80" t="s">
         <v>1438</v>
-      </c>
-      <c r="AX109" s="80" t="s">
-        <v>1439</v>
       </c>
       <c r="BB109" s="58" t="s">
         <v>328</v>
@@ -42565,16 +42622,16 @@
         <v>369</v>
       </c>
       <c r="AU110" s="139" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
       <c r="AV110" s="216">
         <v>43704</v>
       </c>
       <c r="AW110" s="218" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="AX110" s="62" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="111" spans="2:54" ht="89.25" x14ac:dyDescent="0.2">
@@ -42718,10 +42775,10 @@
         <v>43704</v>
       </c>
       <c r="AW111" s="218" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
       <c r="AX111" s="62" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="BB111" s="238" t="s">
         <v>320</v>
@@ -42868,10 +42925,10 @@
         <v>43706</v>
       </c>
       <c r="AW112" s="218" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="AX112" s="62" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
       <c r="BB112" s="61" t="s">
         <v>1029</v>
@@ -43018,13 +43075,13 @@
         <v>43706</v>
       </c>
       <c r="AW113" s="218" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
       <c r="AX113" s="62" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="AY113" s="80" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
       <c r="BB113" s="61" t="s">
         <v>1012</v>
@@ -43171,13 +43228,13 @@
         <v>43706</v>
       </c>
       <c r="AW114" s="218" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
       <c r="AX114" s="80" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="AY114" s="80" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
       <c r="BB114" s="58" t="s">
         <v>1025</v>
@@ -43324,13 +43381,13 @@
         <v>43706</v>
       </c>
       <c r="AW115" s="218" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
       <c r="AX115" s="62" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
       <c r="AY115" s="80" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="BB115" s="176" t="s">
         <v>328</v>
@@ -43477,13 +43534,13 @@
         <v>43711</v>
       </c>
       <c r="AW116" s="218" t="s">
+        <v>1460</v>
+      </c>
+      <c r="AX116" s="62" t="s">
+        <v>1458</v>
+      </c>
+      <c r="AY116" s="62" t="s">
         <v>1461</v>
-      </c>
-      <c r="AX116" s="62" t="s">
-        <v>1459</v>
-      </c>
-      <c r="AY116" s="62" t="s">
-        <v>1462</v>
       </c>
       <c r="BB116" s="176" t="s">
         <v>324</v>
@@ -43630,10 +43687,10 @@
         <v>43711</v>
       </c>
       <c r="AW117" s="218" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
       <c r="AX117" s="62" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
       <c r="BB117" s="176" t="s">
         <v>328</v>
@@ -43776,16 +43833,16 @@
         <v>369</v>
       </c>
       <c r="AU118" s="139" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
       <c r="AV118" s="216">
         <v>43711</v>
       </c>
       <c r="AW118" s="218" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
       <c r="AX118" s="62" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
       <c r="BB118" s="242" t="s">
         <v>321</v>
@@ -43928,16 +43985,16 @@
         <v>369</v>
       </c>
       <c r="AU119" s="241" t="s">
-        <v>1472</v>
+        <v>1471</v>
       </c>
       <c r="AV119" s="216">
         <v>43711</v>
       </c>
       <c r="AW119" s="218" t="s">
-        <v>1466</v>
+        <v>1465</v>
       </c>
       <c r="AX119" s="62" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
       <c r="BB119" s="176" t="s">
         <v>324</v>
@@ -44080,16 +44137,16 @@
         <v>369</v>
       </c>
       <c r="AU120" s="243" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
       <c r="AV120" s="216">
         <v>43713</v>
       </c>
       <c r="AW120" s="218" t="s">
-        <v>1471</v>
+        <v>1470</v>
       </c>
       <c r="AX120" s="80" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
       <c r="BB120" s="244" t="s">
         <v>1031</v>
@@ -44232,7 +44289,7 @@
         <v>369</v>
       </c>
       <c r="AU121" s="139" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
       <c r="AV121" s="216">
         <v>43713</v>
@@ -44240,7 +44297,7 @@
       <c r="AW121" s="231"/>
       <c r="AX121" s="62"/>
       <c r="AY121" s="62" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
       <c r="BB121" s="61" t="s">
         <v>1030</v>
@@ -44377,16 +44434,16 @@
         <v>369</v>
       </c>
       <c r="AU122" s="139" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
       <c r="AV122" s="216">
         <v>43713</v>
       </c>
       <c r="AW122" s="218" t="s">
+        <v>1474</v>
+      </c>
+      <c r="AX122" s="62" t="s">
         <v>1475</v>
-      </c>
-      <c r="AX122" s="62" t="s">
-        <v>1476</v>
       </c>
       <c r="AY122" s="62" t="s">
         <v>1033</v>
@@ -44536,13 +44593,13 @@
         <v>43713</v>
       </c>
       <c r="AW123" s="218" t="s">
+        <v>1477</v>
+      </c>
+      <c r="AX123" s="62" t="s">
+        <v>1476</v>
+      </c>
+      <c r="AY123" s="62" t="s">
         <v>1478</v>
-      </c>
-      <c r="AX123" s="62" t="s">
-        <v>1477</v>
-      </c>
-      <c r="AY123" s="62" t="s">
-        <v>1479</v>
       </c>
     </row>
     <row r="124" spans="2:54" ht="114.75" x14ac:dyDescent="0.2">
@@ -44644,13 +44701,13 @@
         <v>43713</v>
       </c>
       <c r="AW124" s="218" t="s">
+        <v>1480</v>
+      </c>
+      <c r="AX124" s="62" t="s">
+        <v>1479</v>
+      </c>
+      <c r="AY124" s="62" t="s">
         <v>1481</v>
-      </c>
-      <c r="AX124" s="62" t="s">
-        <v>1480</v>
-      </c>
-      <c r="AY124" s="62" t="s">
-        <v>1482</v>
       </c>
     </row>
     <row r="125" spans="2:54" ht="63.75" x14ac:dyDescent="0.2">
@@ -44746,7 +44803,7 @@
       <c r="AS125" s="23"/>
       <c r="AT125" s="24"/>
       <c r="AU125" s="139" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="AV125" s="216">
         <v>43713</v>
@@ -44859,10 +44916,10 @@
         <v>43713</v>
       </c>
       <c r="AW126" s="218" t="s">
+        <v>1482</v>
+      </c>
+      <c r="AX126" s="62" t="s">
         <v>1483</v>
-      </c>
-      <c r="AX126" s="62" t="s">
-        <v>1484</v>
       </c>
       <c r="BB126" s="61" t="s">
         <v>324</v>
@@ -44965,10 +45022,10 @@
         <v>43713</v>
       </c>
       <c r="AW127" s="218" t="s">
+        <v>1484</v>
+      </c>
+      <c r="AX127" s="62" t="s">
         <v>1485</v>
-      </c>
-      <c r="AX127" s="62" t="s">
-        <v>1486</v>
       </c>
       <c r="AY127" s="80" t="s">
         <v>1035</v>
@@ -45114,7 +45171,7 @@
       <c r="AU128" s="139"/>
       <c r="AW128" s="79"/>
     </row>
-    <row r="129" spans="2:54" ht="51" x14ac:dyDescent="0.2">
+    <row r="129" spans="2:55" ht="51" x14ac:dyDescent="0.2">
       <c r="B129" s="21" t="s">
         <v>207</v>
       </c>
@@ -45203,11 +45260,11 @@
       <c r="AS129" s="23"/>
       <c r="AT129" s="24"/>
       <c r="AU129" s="139" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
       <c r="AW129" s="79"/>
     </row>
-    <row r="130" spans="2:54" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="130" spans="2:55" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B130" s="21" t="s">
         <v>208</v>
       </c>
@@ -45308,11 +45365,11 @@
       <c r="AS130" s="23"/>
       <c r="AT130" s="24"/>
       <c r="AU130" s="139" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
       <c r="AW130" s="79"/>
     </row>
-    <row r="131" spans="2:54" s="105" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="131" spans="2:55" s="105" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
       <c r="B131" s="95" t="s">
         <v>208</v>
       </c>
@@ -45402,13 +45459,13 @@
       <c r="AT131" s="101"/>
       <c r="AU131" s="139"/>
       <c r="AV131" s="225" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
       <c r="AW131" s="154" t="s">
+        <v>1488</v>
+      </c>
+      <c r="AX131" s="69" t="s">
         <v>1489</v>
-      </c>
-      <c r="AX131" s="69" t="s">
-        <v>1490</v>
       </c>
       <c r="AY131" s="70"/>
       <c r="AZ131" s="66"/>
@@ -45416,8 +45473,9 @@
       <c r="BB131" s="66" t="s">
         <v>321</v>
       </c>
+      <c r="BC131" s="286"/>
     </row>
-    <row r="132" spans="2:54" s="105" customFormat="1" ht="96.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="2:55" s="105" customFormat="1" ht="96.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B132" s="95" t="s">
         <v>208</v>
       </c>
@@ -45507,13 +45565,13 @@
       <c r="AT132" s="101"/>
       <c r="AU132" s="139"/>
       <c r="AV132" s="225" t="s">
+        <v>1490</v>
+      </c>
+      <c r="AW132" s="167" t="s">
         <v>1491</v>
       </c>
-      <c r="AW132" s="167" t="s">
+      <c r="AX132" s="69" t="s">
         <v>1492</v>
-      </c>
-      <c r="AX132" s="69" t="s">
-        <v>1493</v>
       </c>
       <c r="AY132" s="70"/>
       <c r="AZ132" s="66"/>
@@ -45521,8 +45579,9 @@
       <c r="BB132" s="66" t="s">
         <v>321</v>
       </c>
+      <c r="BC132" s="286"/>
     </row>
-    <row r="133" spans="2:54" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="133" spans="2:55" ht="140.25" x14ac:dyDescent="0.2">
       <c r="B133" s="21" t="s">
         <v>206</v>
       </c>
@@ -45661,7 +45720,7 @@
       <c r="AU133" s="139"/>
       <c r="AW133" s="79"/>
     </row>
-    <row r="134" spans="2:54" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="134" spans="2:55" ht="76.5" x14ac:dyDescent="0.2">
       <c r="B134" s="21" t="s">
         <v>207</v>
       </c>
@@ -45800,7 +45859,7 @@
       <c r="AU134" s="139"/>
       <c r="AW134" s="79"/>
     </row>
-    <row r="135" spans="2:54" ht="249.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="2:55" ht="249.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B135" s="21" t="s">
         <v>207</v>
       </c>
@@ -45937,22 +45996,22 @@
         <v>369</v>
       </c>
       <c r="AU135" s="153" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
       <c r="AV135" s="235" t="s">
+        <v>1495</v>
+      </c>
+      <c r="AW135" s="218" t="s">
         <v>1496</v>
       </c>
-      <c r="AW135" s="218" t="s">
+      <c r="AX135" s="62" t="s">
         <v>1497</v>
-      </c>
-      <c r="AX135" s="62" t="s">
-        <v>1498</v>
       </c>
       <c r="BB135" s="61" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="136" spans="2:54" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="136" spans="2:55" ht="127.5" x14ac:dyDescent="0.2">
       <c r="B136" s="21" t="s">
         <v>207</v>
       </c>
@@ -46089,25 +46148,25 @@
         <v>369</v>
       </c>
       <c r="AU136" s="139" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
       <c r="AV136" s="216">
         <v>43718</v>
       </c>
       <c r="AW136" s="63" t="s">
+        <v>1501</v>
+      </c>
+      <c r="AX136" s="62" t="s">
         <v>1502</v>
       </c>
-      <c r="AX136" s="62" t="s">
-        <v>1503</v>
-      </c>
       <c r="AY136" s="62" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
       <c r="BB136" s="61" t="s">
         <v>976</v>
       </c>
     </row>
-    <row r="137" spans="2:54" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="137" spans="2:55" ht="89.25" x14ac:dyDescent="0.2">
       <c r="B137" s="21" t="s">
         <v>207</v>
       </c>
@@ -46244,25 +46303,25 @@
         <v>369</v>
       </c>
       <c r="AU137" s="139" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="AV137" s="216">
         <v>43720</v>
       </c>
-      <c r="AW137" s="284" t="s">
-        <v>1504</v>
+      <c r="AW137" s="248" t="s">
+        <v>1503</v>
       </c>
       <c r="AX137" s="80" t="s">
+        <v>1505</v>
+      </c>
+      <c r="AY137" s="80" t="s">
         <v>1506</v>
-      </c>
-      <c r="AY137" s="80" t="s">
-        <v>1507</v>
       </c>
       <c r="BB137" s="58" t="s">
         <v>976</v>
       </c>
     </row>
-    <row r="138" spans="2:54" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="138" spans="2:55" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B138" s="21" t="s">
         <v>207</v>
       </c>
@@ -46399,25 +46458,25 @@
         <v>369</v>
       </c>
       <c r="AU138" s="139" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="AV138" s="216">
         <v>43720</v>
       </c>
-      <c r="AW138" s="284" t="s">
+      <c r="AW138" s="248" t="s">
+        <v>1507</v>
+      </c>
+      <c r="AX138" s="80" t="s">
         <v>1508</v>
       </c>
-      <c r="AX138" s="80" t="s">
+      <c r="AY138" s="80" t="s">
         <v>1509</v>
-      </c>
-      <c r="AY138" s="80" t="s">
-        <v>1510</v>
       </c>
       <c r="BB138" s="61" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="139" spans="2:54" ht="105" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:55" ht="105" x14ac:dyDescent="0.25">
       <c r="B139" s="21" t="s">
         <v>207</v>
       </c>
@@ -46509,22 +46568,22 @@
         <v>1274</v>
       </c>
       <c r="AV139" s="230" t="s">
+        <v>1511</v>
+      </c>
+      <c r="AW139" s="249" t="s">
         <v>1512</v>
       </c>
-      <c r="AW139" s="285" t="s">
+      <c r="AX139" s="62" t="s">
         <v>1513</v>
       </c>
-      <c r="AX139" s="62" t="s">
+      <c r="AY139" s="62" t="s">
         <v>1514</v>
-      </c>
-      <c r="AY139" s="62" t="s">
-        <v>1515</v>
       </c>
       <c r="BB139" s="61" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="140" spans="2:54" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="140" spans="2:55" ht="89.25" x14ac:dyDescent="0.2">
       <c r="B140" s="21" t="s">
         <v>206</v>
       </c>
@@ -46636,7 +46695,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="141" spans="2:54" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="141" spans="2:55" ht="76.5" x14ac:dyDescent="0.2">
       <c r="B141" s="21" t="s">
         <v>207</v>
       </c>
@@ -46776,17 +46835,17 @@
       <c r="AV141" s="216">
         <v>43720</v>
       </c>
-      <c r="AW141" s="285" t="s">
-        <v>1516</v>
+      <c r="AW141" s="249" t="s">
+        <v>1515</v>
       </c>
       <c r="AX141" s="62" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="BB141" s="246" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="142" spans="2:54" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="142" spans="2:55" ht="127.5" x14ac:dyDescent="0.2">
       <c r="B142" s="21" t="s">
         <v>207</v>
       </c>
@@ -46887,19 +46946,19 @@
         <v>371</v>
       </c>
       <c r="AU142" s="245" t="s">
-        <v>1517</v>
+        <v>1516</v>
       </c>
       <c r="AV142" s="216">
         <v>43720</v>
       </c>
-      <c r="AW142" s="285" t="s">
+      <c r="AW142" s="249" t="s">
+        <v>1517</v>
+      </c>
+      <c r="AX142" s="62" t="s">
         <v>1518</v>
       </c>
-      <c r="AX142" s="62" t="s">
+      <c r="AY142" s="80" t="s">
         <v>1519</v>
-      </c>
-      <c r="AY142" s="80" t="s">
-        <v>1520</v>
       </c>
       <c r="AZ142" s="247"/>
       <c r="BA142" s="247"/>
@@ -46907,7 +46966,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="143" spans="2:54" ht="165.75" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:55" ht="165.75" x14ac:dyDescent="0.25">
       <c r="B143" s="21" t="s">
         <v>207</v>
       </c>
@@ -47002,16 +47061,16 @@
         <v>371</v>
       </c>
       <c r="AU143" s="151" t="s">
+        <v>1520</v>
+      </c>
+      <c r="AV143" s="230" t="s">
         <v>1521</v>
       </c>
-      <c r="AV143" s="230" t="s">
-        <v>1522</v>
-      </c>
-      <c r="AW143" s="285" t="s">
-        <v>1525</v>
+      <c r="AW143" s="249" t="s">
+        <v>1524</v>
       </c>
       <c r="AX143" s="62" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
       <c r="AY143" s="62" t="s">
         <v>1266</v>
@@ -47020,7 +47079,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="144" spans="2:54" ht="90" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:55" ht="90" x14ac:dyDescent="0.25">
       <c r="B144" s="21" t="s">
         <v>207</v>
       </c>
@@ -47157,16 +47216,16 @@
         <v>371</v>
       </c>
       <c r="AU144" s="151" t="s">
+        <v>1522</v>
+      </c>
+      <c r="AV144" s="230" t="s">
         <v>1523</v>
       </c>
-      <c r="AV144" s="230" t="s">
-        <v>1524</v>
-      </c>
-      <c r="AW144" s="285" t="s">
-        <v>1530</v>
+      <c r="AW144" s="249" t="s">
+        <v>1529</v>
       </c>
       <c r="AX144" s="62" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
       <c r="AY144" s="62" t="s">
         <v>737</v>
@@ -47176,7 +47235,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="145" spans="2:54" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="145" spans="2:55" ht="140.25" x14ac:dyDescent="0.2">
       <c r="B145" s="21" t="s">
         <v>207</v>
       </c>
@@ -47316,21 +47375,21 @@
       <c r="AV145" s="216">
         <v>43720</v>
       </c>
-      <c r="AW145" s="285" t="s">
-        <v>1529</v>
+      <c r="AW145" s="249" t="s">
+        <v>1528</v>
       </c>
       <c r="AX145" s="62" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
       <c r="AY145" s="62" t="s">
-        <v>1528</v>
+        <v>1527</v>
       </c>
       <c r="AZ145" s="177"/>
       <c r="BB145" s="246" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="146" spans="2:54" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="146" spans="2:55" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B146" s="21" t="s">
         <v>207</v>
       </c>
@@ -47428,21 +47487,21 @@
       <c r="AV146" s="216">
         <v>43720</v>
       </c>
-      <c r="AW146" s="285" t="s">
+      <c r="AW146" s="249" t="s">
+        <v>1531</v>
+      </c>
+      <c r="AX146" s="62" t="s">
+        <v>1536</v>
+      </c>
+      <c r="AY146" s="62" t="s">
         <v>1532</v>
-      </c>
-      <c r="AX146" s="62" t="s">
-        <v>1537</v>
-      </c>
-      <c r="AY146" s="62" t="s">
-        <v>1533</v>
       </c>
       <c r="AZ146" s="177"/>
       <c r="BB146" s="246" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="147" spans="2:54" ht="165.75" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:55" ht="165.75" x14ac:dyDescent="0.25">
       <c r="B147" s="21" t="s">
         <v>207</v>
       </c>
@@ -47579,16 +47638,16 @@
         <v>371</v>
       </c>
       <c r="AU147" s="151" t="s">
+        <v>1533</v>
+      </c>
+      <c r="AV147" s="230" t="s">
         <v>1534</v>
       </c>
-      <c r="AV147" s="230" t="s">
+      <c r="AW147" s="63" t="s">
         <v>1535</v>
       </c>
-      <c r="AW147" s="63" t="s">
-        <v>1536</v>
-      </c>
       <c r="AX147" s="62" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
       <c r="AY147" s="62" t="s">
         <v>1267</v>
@@ -47597,7 +47656,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="148" spans="2:54" ht="51" x14ac:dyDescent="0.2">
+    <row r="148" spans="2:55" ht="51" x14ac:dyDescent="0.2">
       <c r="B148" s="21" t="s">
         <v>207</v>
       </c>
@@ -47695,20 +47754,20 @@
       <c r="AV148" s="216">
         <v>43720</v>
       </c>
-      <c r="AW148" s="285" t="s">
+      <c r="AW148" s="249" t="s">
+        <v>1538</v>
+      </c>
+      <c r="AX148" s="62" t="s">
         <v>1539</v>
       </c>
-      <c r="AX148" s="62" t="s">
+      <c r="AY148" s="62" t="s">
         <v>1540</v>
-      </c>
-      <c r="AY148" s="62" t="s">
-        <v>1541</v>
       </c>
       <c r="BB148" s="61" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="149" spans="2:54" ht="51" x14ac:dyDescent="0.2">
+    <row r="149" spans="2:55" ht="51" x14ac:dyDescent="0.2">
       <c r="B149" s="21" t="s">
         <v>207</v>
       </c>
@@ -47806,20 +47865,20 @@
       <c r="AV149" s="216">
         <v>43720</v>
       </c>
-      <c r="AW149" s="285" t="s">
+      <c r="AW149" s="249" t="s">
+        <v>1542</v>
+      </c>
+      <c r="AX149" s="62" t="s">
         <v>1543</v>
       </c>
-      <c r="AX149" s="62" t="s">
-        <v>1544</v>
-      </c>
       <c r="AY149" s="62" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
       <c r="BB149" s="61" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="150" spans="2:54" s="116" customFormat="1" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="150" spans="2:55" s="116" customFormat="1" ht="409.5" x14ac:dyDescent="0.2">
       <c r="B150" s="106" t="s">
         <v>207</v>
       </c>
@@ -47934,15 +47993,18 @@
         <v>20190328</v>
       </c>
       <c r="AW150" s="86" t="s">
-        <v>1276</v>
+        <v>1544</v>
       </c>
       <c r="AX150" s="87"/>
       <c r="AY150" s="88"/>
       <c r="AZ150" s="89"/>
       <c r="BA150" s="89"/>
       <c r="BB150" s="90"/>
+      <c r="BC150" s="286" t="s">
+        <v>1545</v>
+      </c>
     </row>
-    <row r="151" spans="2:54" s="116" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="151" spans="2:55" s="116" customFormat="1" ht="153" x14ac:dyDescent="0.2">
       <c r="B151" s="106" t="s">
         <v>207</v>
       </c>
@@ -48096,8 +48158,11 @@
       <c r="BB151" s="90" t="s">
         <v>1041</v>
       </c>
+      <c r="BC151" s="286" t="s">
+        <v>1546</v>
+      </c>
     </row>
-    <row r="152" spans="2:54" s="116" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="152" spans="2:55" s="116" customFormat="1" ht="153" x14ac:dyDescent="0.2">
       <c r="B152" s="106" t="s">
         <v>207</v>
       </c>
@@ -48207,8 +48272,11 @@
       <c r="BB152" s="90" t="s">
         <v>1041</v>
       </c>
+      <c r="BC152" s="286" t="s">
+        <v>1547</v>
+      </c>
     </row>
-    <row r="153" spans="2:54" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="153" spans="2:55" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B153" s="21" t="s">
         <v>206</v>
       </c>
@@ -48340,8 +48408,11 @@
       <c r="AT153" s="24"/>
       <c r="AU153" s="139"/>
       <c r="AW153" s="79"/>
+      <c r="BC153" s="286" t="s">
+        <v>1548</v>
+      </c>
     </row>
-    <row r="154" spans="2:54" ht="51" x14ac:dyDescent="0.2">
+    <row r="154" spans="2:55" ht="89.25" x14ac:dyDescent="0.2">
       <c r="B154" s="21" t="s">
         <v>207</v>
       </c>
@@ -48473,8 +48544,11 @@
       <c r="AT154" s="24"/>
       <c r="AU154" s="139"/>
       <c r="AW154" s="79"/>
+      <c r="BC154" s="286" t="s">
+        <v>1549</v>
+      </c>
     </row>
-    <row r="155" spans="2:54" ht="51" x14ac:dyDescent="0.2">
+    <row r="155" spans="2:55" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B155" s="21" t="s">
         <v>207</v>
       </c>
@@ -48615,8 +48689,11 @@
       <c r="BB155" s="58" t="s">
         <v>976</v>
       </c>
+      <c r="BC155" s="286" t="s">
+        <v>1548</v>
+      </c>
     </row>
-    <row r="156" spans="2:54" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="156" spans="2:55" ht="216.75" x14ac:dyDescent="0.2">
       <c r="B156" s="21" t="s">
         <v>208</v>
       </c>
@@ -48754,7 +48831,7 @@
       </c>
       <c r="AW156" s="82"/>
       <c r="AX156" s="62" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="AY156" s="68" t="s">
         <v>1000</v>
@@ -48762,8 +48839,11 @@
       <c r="BB156" s="61" t="s">
         <v>1030</v>
       </c>
+      <c r="BC156" s="286" t="s">
+        <v>1550</v>
+      </c>
     </row>
-    <row r="157" spans="2:54" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="157" spans="2:55" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B157" s="21" t="s">
         <v>208</v>
       </c>
@@ -48885,8 +48965,11 @@
       <c r="AW157" s="82" t="s">
         <v>1046</v>
       </c>
+      <c r="BC157" s="286" t="s">
+        <v>1551</v>
+      </c>
     </row>
-    <row r="158" spans="2:54" x14ac:dyDescent="0.2">
+    <row r="158" spans="2:55" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B158" s="21" t="s">
         <v>208</v>
       </c>
@@ -49018,8 +49101,11 @@
       <c r="AT158" s="24"/>
       <c r="AU158" s="139"/>
       <c r="AW158" s="79"/>
+      <c r="BC158" s="286" t="s">
+        <v>1552</v>
+      </c>
     </row>
-    <row r="159" spans="2:54" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="159" spans="2:55" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B159" s="21" t="s">
         <v>208</v>
       </c>
@@ -49139,8 +49225,11 @@
       <c r="AT159" s="24"/>
       <c r="AU159" s="139"/>
       <c r="AW159" s="79"/>
+      <c r="BC159" s="286" t="s">
+        <v>1553</v>
+      </c>
     </row>
-    <row r="160" spans="2:54" x14ac:dyDescent="0.2">
+    <row r="160" spans="2:55" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B160" s="21" t="s">
         <v>209</v>
       </c>
@@ -49277,8 +49366,11 @@
         <v>20190326</v>
       </c>
       <c r="AW160" s="79"/>
+      <c r="BC160" s="286" t="s">
+        <v>1553</v>
+      </c>
     </row>
-    <row r="161" spans="2:54" s="105" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="161" spans="2:55" s="105" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B161" s="95" t="s">
         <v>209</v>
       </c>
@@ -49414,8 +49506,11 @@
       <c r="BB161" s="66" t="s">
         <v>321</v>
       </c>
+      <c r="BC161" s="286" t="s">
+        <v>1554</v>
+      </c>
     </row>
-    <row r="162" spans="2:54" s="105" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="162" spans="2:55" s="105" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B162" s="95" t="s">
         <v>209</v>
       </c>
@@ -49551,8 +49646,11 @@
       <c r="BB162" s="66" t="s">
         <v>321</v>
       </c>
+      <c r="BC162" s="286" t="s">
+        <v>1555</v>
+      </c>
     </row>
-    <row r="163" spans="2:54" s="105" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="163" spans="2:55" s="105" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="B163" s="95" t="s">
         <v>209</v>
       </c>
@@ -49688,8 +49786,11 @@
       <c r="BB163" s="66" t="s">
         <v>321</v>
       </c>
+      <c r="BC163" s="286" t="s">
+        <v>1555</v>
+      </c>
     </row>
-    <row r="164" spans="2:54" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="164" spans="2:55" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B164" s="21" t="s">
         <v>207</v>
       </c>
@@ -49821,8 +49922,11 @@
       <c r="AT164" s="24"/>
       <c r="AU164" s="139"/>
       <c r="AW164" s="79"/>
+      <c r="BC164" s="286" t="s">
+        <v>323</v>
+      </c>
     </row>
-    <row r="165" spans="2:54" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="165" spans="2:55" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B165" s="21" t="s">
         <v>207</v>
       </c>
@@ -49942,8 +50046,11 @@
       <c r="AT165" s="24"/>
       <c r="AU165" s="139"/>
       <c r="AW165" s="79"/>
+      <c r="BC165" s="286" t="s">
+        <v>323</v>
+      </c>
     </row>
-    <row r="166" spans="2:54" ht="153" x14ac:dyDescent="0.2">
+    <row r="166" spans="2:55" ht="153" x14ac:dyDescent="0.2">
       <c r="B166" s="21" t="s">
         <v>206</v>
       </c>
@@ -50081,8 +50188,11 @@
       </c>
       <c r="AU166" s="139"/>
       <c r="AW166" s="79"/>
+      <c r="BC166" s="286" t="s">
+        <v>1556</v>
+      </c>
     </row>
-    <row r="167" spans="2:54" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="167" spans="2:55" ht="89.25" x14ac:dyDescent="0.2">
       <c r="B167" s="21" t="s">
         <v>207</v>
       </c>
@@ -50218,8 +50328,11 @@
       </c>
       <c r="AU167" s="139"/>
       <c r="AW167" s="79"/>
+      <c r="BC167" s="286" t="s">
+        <v>1557</v>
+      </c>
     </row>
-    <row r="168" spans="2:54" s="105" customFormat="1" ht="150" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="2:55" s="105" customFormat="1" ht="150" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B168" s="95" t="s">
         <v>207</v>
       </c>
@@ -50355,8 +50468,11 @@
       <c r="AZ168" s="66"/>
       <c r="BA168" s="66"/>
       <c r="BB168" s="66"/>
+      <c r="BC168" s="286" t="s">
+        <v>1558</v>
+      </c>
     </row>
-    <row r="169" spans="2:54" ht="183.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="2:55" ht="183.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B169" s="21" t="s">
         <v>207</v>
       </c>
@@ -50450,8 +50566,11 @@
       <c r="AV169" s="154" t="s">
         <v>1186</v>
       </c>
+      <c r="BC169" s="286" t="s">
+        <v>1559</v>
+      </c>
     </row>
-    <row r="170" spans="2:54" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="170" spans="2:55" ht="140.25" x14ac:dyDescent="0.2">
       <c r="B170" s="21" t="s">
         <v>207</v>
       </c>
@@ -50598,8 +50717,11 @@
       <c r="BB170" s="61" t="s">
         <v>1012</v>
       </c>
+      <c r="BC170" s="286" t="s">
+        <v>1559</v>
+      </c>
     </row>
-    <row r="171" spans="2:54" ht="77.25" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:55" ht="127.5" x14ac:dyDescent="0.25">
       <c r="B171" s="21" t="s">
         <v>207</v>
       </c>
@@ -50753,8 +50875,11 @@
       <c r="BB171" s="61" t="s">
         <v>324</v>
       </c>
+      <c r="BC171" s="286" t="s">
+        <v>1560</v>
+      </c>
     </row>
-    <row r="172" spans="2:54" ht="240" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:55" ht="240" x14ac:dyDescent="0.25">
       <c r="B172" s="21" t="s">
         <v>207</v>
       </c>
@@ -50898,7 +51023,7 @@
       </c>
       <c r="AW172" s="79"/>
     </row>
-    <row r="173" spans="2:54" s="105" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="173" spans="2:55" s="105" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
       <c r="B173" s="95" t="s">
         <v>207</v>
       </c>
@@ -51020,8 +51145,9 @@
       <c r="BB173" s="67" t="s">
         <v>976</v>
       </c>
+      <c r="BC173" s="286"/>
     </row>
-    <row r="174" spans="2:54" ht="195" x14ac:dyDescent="0.2">
+    <row r="174" spans="2:55" ht="195" x14ac:dyDescent="0.2">
       <c r="B174" s="21" t="s">
         <v>207</v>
       </c>
@@ -51176,7 +51302,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="175" spans="2:54" s="105" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="175" spans="2:55" s="105" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B175" s="95" t="s">
         <v>207</v>
       </c>
@@ -51296,8 +51422,9 @@
       <c r="BB175" s="67" t="s">
         <v>976</v>
       </c>
+      <c r="BC175" s="286"/>
     </row>
-    <row r="176" spans="2:54" s="116" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:55" s="116" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="B176" s="106" t="s">
         <v>207</v>
       </c>
@@ -51445,8 +51572,9 @@
       <c r="AZ176" s="89"/>
       <c r="BA176" s="89"/>
       <c r="BB176" s="89"/>
+      <c r="BC176" s="286"/>
     </row>
-    <row r="177" spans="2:54" s="116" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:55" s="116" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B177" s="106" t="s">
         <v>207</v>
       </c>
@@ -51588,8 +51716,9 @@
       <c r="AZ177" s="89"/>
       <c r="BA177" s="89"/>
       <c r="BB177" s="89"/>
+      <c r="BC177" s="286"/>
     </row>
-    <row r="178" spans="2:54" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="178" spans="2:55" ht="89.25" x14ac:dyDescent="0.2">
       <c r="B178" s="21" t="s">
         <v>206</v>
       </c>
@@ -51728,7 +51857,7 @@
       <c r="AU178" s="139"/>
       <c r="AW178" s="79"/>
     </row>
-    <row r="179" spans="2:54" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="179" spans="2:55" ht="89.25" x14ac:dyDescent="0.2">
       <c r="B179" s="21" t="s">
         <v>207</v>
       </c>
@@ -51867,7 +51996,7 @@
       <c r="AU179" s="139"/>
       <c r="AW179" s="79"/>
     </row>
-    <row r="180" spans="2:54" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="180" spans="2:55" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B180" s="21" t="s">
         <v>207</v>
       </c>
@@ -52009,7 +52138,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="181" spans="2:54" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="181" spans="2:55" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B181" s="21" t="s">
         <v>207</v>
       </c>
@@ -52150,7 +52279,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="182" spans="2:54" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="182" spans="2:55" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B182" s="21" t="s">
         <v>207</v>
       </c>
@@ -52289,7 +52418,7 @@
       <c r="AU182" s="139"/>
       <c r="AW182" s="79"/>
     </row>
-    <row r="183" spans="2:54" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="183" spans="2:55" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B183" s="21" t="s">
         <v>207</v>
       </c>
@@ -52428,7 +52557,7 @@
       <c r="AU183" s="139"/>
       <c r="AW183" s="79"/>
     </row>
-    <row r="184" spans="2:54" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="184" spans="2:55" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B184" s="21" t="s">
         <v>207</v>
       </c>
@@ -52567,7 +52696,7 @@
       <c r="AU184" s="139"/>
       <c r="AW184" s="79"/>
     </row>
-    <row r="185" spans="2:54" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="185" spans="2:55" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B185" s="21" t="s">
         <v>207</v>
       </c>
@@ -52714,7 +52843,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="186" spans="2:54" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="186" spans="2:55" ht="89.25" x14ac:dyDescent="0.2">
       <c r="B186" s="21" t="s">
         <v>206</v>
       </c>
@@ -52821,7 +52950,7 @@
       <c r="AU186" s="139"/>
       <c r="AW186" s="79"/>
     </row>
-    <row r="187" spans="2:54" ht="29.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="2:55" ht="29.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B187" s="21" t="s">
         <v>207</v>
       </c>
@@ -52928,7 +53057,7 @@
       <c r="AU187" s="139"/>
       <c r="AW187" s="79"/>
     </row>
-    <row r="188" spans="2:54" ht="153" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:55" ht="153" x14ac:dyDescent="0.25">
       <c r="B188" s="21" t="s">
         <v>207</v>
       </c>
@@ -53080,7 +53209,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="189" spans="2:54" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="189" spans="2:55" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B189" s="21" t="s">
         <v>207</v>
       </c>
@@ -53233,7 +53362,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="190" spans="2:54" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="2:55" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B190" s="21" t="s">
         <v>207</v>
       </c>
@@ -53354,7 +53483,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="191" spans="2:54" ht="150" x14ac:dyDescent="0.2">
+    <row r="191" spans="2:55" ht="150" x14ac:dyDescent="0.2">
       <c r="B191" s="21" t="s">
         <v>207</v>
       </c>
@@ -53506,7 +53635,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="192" spans="2:54" ht="270" x14ac:dyDescent="0.2">
+    <row r="192" spans="2:55" ht="270" x14ac:dyDescent="0.2">
       <c r="B192" s="21" t="s">
         <v>207</v>
       </c>
@@ -53650,7 +53779,7 @@
       </c>
       <c r="AW192" s="79"/>
     </row>
-    <row r="193" spans="2:54" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="2:55" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B193" s="21" t="s">
         <v>207</v>
       </c>
@@ -53787,14 +53916,14 @@
         <v>369</v>
       </c>
       <c r="AU193" s="135" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="AV193" s="138">
         <v>20190307</v>
       </c>
       <c r="AW193" s="79"/>
     </row>
-    <row r="194" spans="2:54" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:55" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B194" s="21" t="s">
         <v>207</v>
       </c>
@@ -53946,7 +54075,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="195" spans="2:54" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="2:55" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B195" s="21" t="s">
         <v>206</v>
       </c>
@@ -54041,7 +54170,7 @@
       <c r="AU195" s="139"/>
       <c r="AW195" s="79"/>
     </row>
-    <row r="196" spans="2:54" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="2:55" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B196" s="21" t="s">
         <v>207</v>
       </c>
@@ -54152,7 +54281,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="197" spans="2:54" ht="102" x14ac:dyDescent="0.2">
+    <row r="197" spans="2:55" ht="102" x14ac:dyDescent="0.2">
       <c r="B197" s="21" t="s">
         <v>207</v>
       </c>
@@ -54296,7 +54425,7 @@
       </c>
       <c r="AW197" s="82"/>
       <c r="AX197" s="62" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="AY197" s="180" t="s">
         <v>1000</v>
@@ -54305,7 +54434,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="198" spans="2:54" ht="282.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="2:55" ht="282.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B198" s="21" t="s">
         <v>207</v>
       </c>
@@ -54449,7 +54578,7 @@
       </c>
       <c r="AW198" s="82"/>
       <c r="AX198" s="62" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="AY198" s="180" t="s">
         <v>1000</v>
@@ -54458,7 +54587,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="199" spans="2:54" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="199" spans="2:55" ht="140.25" x14ac:dyDescent="0.2">
       <c r="B199" s="21" t="s">
         <v>207</v>
       </c>
@@ -54566,7 +54695,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="200" spans="2:54" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="200" spans="2:55" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B200" s="21" t="s">
         <v>207</v>
       </c>
@@ -54705,7 +54834,7 @@
       <c r="AU200" s="139"/>
       <c r="AW200" s="79"/>
     </row>
-    <row r="201" spans="2:54" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="201" spans="2:55" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B201" s="21" t="s">
         <v>207</v>
       </c>
@@ -54852,7 +54981,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="202" spans="2:54" s="105" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="202" spans="2:55" s="105" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B202" s="95" t="s">
         <v>207</v>
       </c>
@@ -54942,8 +55071,9 @@
       <c r="AZ202" s="66"/>
       <c r="BA202" s="66"/>
       <c r="BB202" s="66"/>
+      <c r="BC202" s="286"/>
     </row>
-    <row r="203" spans="2:54" ht="216.75" x14ac:dyDescent="0.2">
+    <row r="203" spans="2:55" ht="216.75" x14ac:dyDescent="0.2">
       <c r="B203" s="21" t="s">
         <v>207</v>
       </c>
@@ -55054,7 +55184,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="204" spans="2:54" s="116" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="204" spans="2:55" s="116" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
       <c r="B204" s="106" t="s">
         <v>207</v>
       </c>
@@ -55200,7 +55330,7 @@
         <v>1237</v>
       </c>
       <c r="AX204" s="87" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="AY204" s="88"/>
       <c r="AZ204" s="89"/>
@@ -55208,8 +55338,9 @@
       <c r="BB204" s="90" t="s">
         <v>1030</v>
       </c>
+      <c r="BC204" s="286"/>
     </row>
-    <row r="205" spans="2:54" s="105" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="205" spans="2:55" s="105" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B205" s="95" t="s">
         <v>207</v>
       </c>
@@ -55307,8 +55438,9 @@
       <c r="AZ205" s="66"/>
       <c r="BA205" s="66"/>
       <c r="BB205" s="67"/>
+      <c r="BC205" s="286"/>
     </row>
-    <row r="206" spans="2:54" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="206" spans="2:55" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B206" s="21" t="s">
         <v>207</v>
       </c>
@@ -55454,7 +55586,7 @@
         <v>1069</v>
       </c>
     </row>
-    <row r="207" spans="2:54" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="207" spans="2:55" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B207" s="21" t="s">
         <v>207</v>
       </c>
@@ -55535,7 +55667,7 @@
       <c r="AU207" s="139"/>
       <c r="AW207" s="79"/>
     </row>
-    <row r="208" spans="2:54" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="208" spans="2:55" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B208" s="21" t="s">
         <v>207</v>
       </c>
@@ -55685,7 +55817,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="209" spans="2:54" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="209" spans="2:55" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B209" s="21" t="s">
         <v>207</v>
       </c>
@@ -55835,7 +55967,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="210" spans="2:54" s="116" customFormat="1" ht="191.25" x14ac:dyDescent="0.2">
+    <row r="210" spans="2:55" s="116" customFormat="1" ht="191.25" x14ac:dyDescent="0.2">
       <c r="B210" s="106" t="s">
         <v>207</v>
       </c>
@@ -55939,8 +56071,9 @@
       <c r="BB210" s="90" t="s">
         <v>328</v>
       </c>
+      <c r="BC210" s="286"/>
     </row>
-    <row r="211" spans="2:54" s="116" customFormat="1" ht="135" x14ac:dyDescent="0.2">
+    <row r="211" spans="2:55" s="116" customFormat="1" ht="135" x14ac:dyDescent="0.2">
       <c r="B211" s="106" t="s">
         <v>207</v>
       </c>
@@ -56096,8 +56229,9 @@
       <c r="BB211" s="90" t="s">
         <v>324</v>
       </c>
+      <c r="BC211" s="286"/>
     </row>
-    <row r="212" spans="2:54" s="105" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="212" spans="2:55" s="105" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B212" s="95" t="s">
         <v>207</v>
       </c>
@@ -56175,8 +56309,9 @@
       <c r="BB212" s="67" t="s">
         <v>976</v>
       </c>
+      <c r="BC212" s="286"/>
     </row>
-    <row r="213" spans="2:54" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="213" spans="2:55" ht="76.5" x14ac:dyDescent="0.2">
       <c r="B213" s="21" t="s">
         <v>207</v>
       </c>
@@ -56331,7 +56466,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="214" spans="2:54" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="214" spans="2:55" ht="76.5" x14ac:dyDescent="0.2">
       <c r="B214" s="21" t="s">
         <v>207</v>
       </c>
@@ -56477,13 +56612,13 @@
         <v>1017</v>
       </c>
       <c r="AX214" s="62" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="BB214" s="178" t="s">
         <v>976</v>
       </c>
     </row>
-    <row r="215" spans="2:54" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="215" spans="2:55" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B215" s="21" t="s">
         <v>207</v>
       </c>
@@ -56638,7 +56773,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="216" spans="2:54" s="105" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="2:55" s="105" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B216" s="95" t="s">
         <v>207</v>
       </c>
@@ -56736,8 +56871,9 @@
       <c r="AZ216" s="66"/>
       <c r="BA216" s="66"/>
       <c r="BB216" s="67"/>
+      <c r="BC216" s="286"/>
     </row>
-    <row r="217" spans="2:54" s="105" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="217" spans="2:55" s="105" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B217" s="95" t="s">
         <v>207</v>
       </c>
@@ -56835,8 +56971,9 @@
       <c r="AZ217" s="66"/>
       <c r="BA217" s="66"/>
       <c r="BB217" s="67"/>
+      <c r="BC217" s="286"/>
     </row>
-    <row r="218" spans="2:54" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="218" spans="2:55" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B218" s="21" t="s">
         <v>206</v>
       </c>
@@ -56975,7 +57112,7 @@
       <c r="AU218" s="139"/>
       <c r="AW218" s="79"/>
     </row>
-    <row r="219" spans="2:54" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="219" spans="2:55" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B219" s="21" t="s">
         <v>207</v>
       </c>
@@ -57121,7 +57258,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="220" spans="2:54" ht="51" x14ac:dyDescent="0.2">
+    <row r="220" spans="2:55" ht="51" x14ac:dyDescent="0.2">
       <c r="B220" s="21" t="s">
         <v>207</v>
       </c>
@@ -57267,7 +57404,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="221" spans="2:54" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="221" spans="2:55" ht="89.25" x14ac:dyDescent="0.2">
       <c r="B221" s="21" t="s">
         <v>207</v>
       </c>
@@ -57408,7 +57545,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="222" spans="2:54" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="222" spans="2:55" ht="76.5" x14ac:dyDescent="0.2">
       <c r="B222" s="21" t="s">
         <v>208</v>
       </c>
@@ -57545,22 +57682,22 @@
         <v>371</v>
       </c>
       <c r="AU222" s="93" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="AV222" s="94">
         <v>20190319</v>
       </c>
       <c r="AW222" s="82" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="AX222" s="62" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="BB222" s="176" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="223" spans="2:54" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="223" spans="2:55" ht="140.25" x14ac:dyDescent="0.2">
       <c r="B223" s="21" t="s">
         <v>208</v>
       </c>
@@ -57697,22 +57834,22 @@
         <v>371</v>
       </c>
       <c r="AU223" s="93" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="AV223" s="94">
         <v>20190321</v>
       </c>
       <c r="AW223" s="82" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="AX223" s="62" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="AY223" s="62" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
     </row>
-    <row r="224" spans="2:54" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="224" spans="2:55" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B224" s="21" t="s">
         <v>207</v>
       </c>
@@ -57851,7 +57988,7 @@
       <c r="AU224" s="139"/>
       <c r="AW224" s="79"/>
     </row>
-    <row r="225" spans="2:54" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="225" spans="2:55" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B225" s="21" t="s">
         <v>208</v>
       </c>
@@ -57988,7 +58125,7 @@
         <v>371</v>
       </c>
       <c r="AU225" s="93" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="AV225" s="94">
         <v>20190319</v>
@@ -58001,7 +58138,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="226" spans="2:54" ht="51" x14ac:dyDescent="0.2">
+    <row r="226" spans="2:55" ht="51" x14ac:dyDescent="0.2">
       <c r="B226" s="21" t="s">
         <v>208</v>
       </c>
@@ -58144,13 +58281,13 @@
         <v>1249</v>
       </c>
       <c r="AY226" s="62" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="BB226" s="61" t="s">
         <v>976</v>
       </c>
     </row>
-    <row r="227" spans="2:54" ht="165.75" x14ac:dyDescent="0.2">
+    <row r="227" spans="2:55" ht="165.75" x14ac:dyDescent="0.2">
       <c r="B227" s="21" t="s">
         <v>208</v>
       </c>
@@ -58281,7 +58418,7 @@
       <c r="AS227" s="23"/>
       <c r="AT227" s="24"/>
       <c r="AU227" s="93" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="AV227" s="138">
         <v>20190319</v>
@@ -58293,7 +58430,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="228" spans="2:54" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="228" spans="2:55" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B228" s="21" t="s">
         <v>208</v>
       </c>
@@ -58432,7 +58569,7 @@
       <c r="AU228" s="139"/>
       <c r="AW228" s="79"/>
     </row>
-    <row r="229" spans="2:54" s="105" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="229" spans="2:55" s="105" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B229" s="95" t="s">
         <v>208</v>
       </c>
@@ -58516,8 +58653,9 @@
       <c r="AZ229" s="66"/>
       <c r="BA229" s="66"/>
       <c r="BB229" s="66"/>
+      <c r="BC229" s="286"/>
     </row>
-    <row r="230" spans="2:54" s="105" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="230" spans="2:55" s="105" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B230" s="95" t="s">
         <v>209</v>
       </c>
@@ -58601,8 +58739,9 @@
       <c r="AZ230" s="66"/>
       <c r="BA230" s="66"/>
       <c r="BB230" s="66"/>
+      <c r="BC230" s="286"/>
     </row>
-    <row r="231" spans="2:54" s="105" customFormat="1" ht="242.25" x14ac:dyDescent="0.2">
+    <row r="231" spans="2:55" s="105" customFormat="1" ht="242.25" x14ac:dyDescent="0.2">
       <c r="B231" s="95" t="s">
         <v>209</v>
       </c>
@@ -58686,8 +58825,9 @@
       <c r="AZ231" s="66"/>
       <c r="BA231" s="66"/>
       <c r="BB231" s="66"/>
+      <c r="BC231" s="286"/>
     </row>
-    <row r="232" spans="2:54" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="232" spans="2:55" ht="114.75" x14ac:dyDescent="0.2">
       <c r="B232" s="21" t="s">
         <v>208</v>
       </c>
@@ -58828,7 +58968,7 @@
       </c>
       <c r="AW232" s="79"/>
     </row>
-    <row r="233" spans="2:54" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="233" spans="2:55" ht="114.75" x14ac:dyDescent="0.2">
       <c r="B233" s="21" t="s">
         <v>208</v>
       </c>
@@ -58969,7 +59109,7 @@
       </c>
       <c r="AW233" s="79"/>
     </row>
-    <row r="234" spans="2:54" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="234" spans="2:55" ht="102" x14ac:dyDescent="0.2">
       <c r="B234" s="21" t="s">
         <v>207</v>
       </c>
@@ -59110,7 +59250,7 @@
       </c>
       <c r="AW234" s="79"/>
     </row>
-    <row r="235" spans="2:54" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="235" spans="2:55" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B235" s="21" t="s">
         <v>208</v>
       </c>
@@ -59251,7 +59391,7 @@
       </c>
       <c r="AW235" s="79"/>
     </row>
-    <row r="236" spans="2:54" ht="51" x14ac:dyDescent="0.2">
+    <row r="236" spans="2:55" ht="51" x14ac:dyDescent="0.2">
       <c r="B236" s="21" t="s">
         <v>208</v>
       </c>
@@ -59392,7 +59532,7 @@
       </c>
       <c r="AW236" s="79"/>
     </row>
-    <row r="237" spans="2:54" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="237" spans="2:55" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B237" s="21" t="s">
         <v>208</v>
       </c>
@@ -59533,7 +59673,7 @@
       </c>
       <c r="AW237" s="79"/>
     </row>
-    <row r="238" spans="2:54" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="238" spans="2:55" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B238" s="21" t="s">
         <v>208</v>
       </c>
@@ -59683,7 +59823,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="239" spans="2:54" s="116" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="239" spans="2:55" s="116" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B239" s="106" t="s">
         <v>208</v>
       </c>
@@ -59833,8 +59973,9 @@
       <c r="BB239" s="90" t="s">
         <v>1012</v>
       </c>
+      <c r="BC239" s="286"/>
     </row>
-    <row r="240" spans="2:54" s="116" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="240" spans="2:55" s="116" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B240" s="106" t="s">
         <v>208</v>
       </c>
@@ -59976,8 +60117,9 @@
       <c r="AZ240" s="89"/>
       <c r="BA240" s="89"/>
       <c r="BB240" s="89"/>
+      <c r="BC240" s="286"/>
     </row>
-    <row r="241" spans="2:54" s="116" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="241" spans="2:55" s="116" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="B241" s="106" t="s">
         <v>208</v>
       </c>
@@ -60119,8 +60261,9 @@
       <c r="AZ241" s="89"/>
       <c r="BA241" s="89"/>
       <c r="BB241" s="89"/>
+      <c r="BC241" s="286"/>
     </row>
-    <row r="242" spans="2:54" x14ac:dyDescent="0.2">
+    <row r="242" spans="2:55" x14ac:dyDescent="0.2">
       <c r="B242" s="21" t="s">
         <v>208</v>
       </c>
@@ -60255,7 +60398,7 @@
       </c>
       <c r="AW242" s="79"/>
     </row>
-    <row r="243" spans="2:54" s="116" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="243" spans="2:55" s="116" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B243" s="106" t="s">
         <v>208</v>
       </c>
@@ -60401,8 +60544,9 @@
       <c r="AZ243" s="89"/>
       <c r="BA243" s="89"/>
       <c r="BB243" s="89"/>
+      <c r="BC243" s="286"/>
     </row>
-    <row r="244" spans="2:54" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="244" spans="2:55" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B244" s="21" t="s">
         <v>208</v>
       </c>
@@ -60543,7 +60687,7 @@
       </c>
       <c r="AW244" s="79"/>
     </row>
-    <row r="245" spans="2:54" s="105" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="245" spans="2:55" s="105" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B245" s="95" t="s">
         <v>209</v>
       </c>
@@ -60639,8 +60783,9 @@
       <c r="AZ245" s="66"/>
       <c r="BA245" s="66"/>
       <c r="BB245" s="66"/>
+      <c r="BC245" s="286"/>
     </row>
-    <row r="246" spans="2:54" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="246" spans="2:55" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B246" s="21" t="s">
         <v>209</v>
       </c>
@@ -60746,7 +60891,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="247" spans="2:54" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="247" spans="2:55" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B247" s="21" t="s">
         <v>209</v>
       </c>
@@ -60887,7 +61032,7 @@
       </c>
       <c r="AW247" s="79"/>
     </row>
-    <row r="248" spans="2:54" s="105" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="248" spans="2:55" s="105" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="B248" s="95" t="s">
         <v>209</v>
       </c>
@@ -60987,8 +61132,9 @@
       <c r="AZ248" s="66"/>
       <c r="BA248" s="66"/>
       <c r="BB248" s="66"/>
+      <c r="BC248" s="286"/>
     </row>
-    <row r="249" spans="2:54" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="249" spans="2:55" ht="76.5" x14ac:dyDescent="0.2">
       <c r="B249" s="21" t="s">
         <v>209</v>
       </c>
@@ -61090,7 +61236,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="250" spans="2:54" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="250" spans="2:55" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B250" s="21" t="s">
         <v>209</v>
       </c>
@@ -61242,7 +61388,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="251" spans="2:54" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="251" spans="2:55" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B251" s="21" t="s">
         <v>209</v>
       </c>
@@ -61385,7 +61531,7 @@
         <v>1089</v>
       </c>
     </row>
-    <row r="252" spans="2:54" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="252" spans="2:55" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B252" s="21" t="s">
         <v>207</v>
       </c>
@@ -61524,7 +61670,7 @@
       <c r="AU252" s="139"/>
       <c r="AW252" s="79"/>
     </row>
-    <row r="253" spans="2:54" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="253" spans="2:55" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B253" s="21" t="s">
         <v>208</v>
       </c>
@@ -61663,7 +61809,7 @@
       <c r="AU253" s="139"/>
       <c r="AW253" s="79"/>
     </row>
-    <row r="254" spans="2:54" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="254" spans="2:55" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B254" s="21" t="s">
         <v>208</v>
       </c>
@@ -61802,7 +61948,7 @@
       <c r="AU254" s="139"/>
       <c r="AW254" s="79"/>
     </row>
-    <row r="255" spans="2:54" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="255" spans="2:55" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B255" s="21" t="s">
         <v>208</v>
       </c>
@@ -61952,7 +62098,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="256" spans="2:54" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="256" spans="2:55" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B256" s="21" t="s">
         <v>208</v>
       </c>
@@ -62099,7 +62245,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="257" spans="2:54" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="257" spans="2:55" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B257" s="21" t="s">
         <v>208</v>
       </c>
@@ -62241,7 +62387,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="258" spans="2:54" s="105" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="258" spans="2:55" s="105" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B258" s="95" t="s">
         <v>208</v>
       </c>
@@ -62323,8 +62469,9 @@
       <c r="AZ258" s="66"/>
       <c r="BA258" s="66"/>
       <c r="BB258" s="67"/>
+      <c r="BC258" s="286"/>
     </row>
-    <row r="259" spans="2:54" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="259" spans="2:55" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B259" s="21" t="s">
         <v>208</v>
       </c>
@@ -62465,7 +62612,7 @@
       </c>
       <c r="AW259" s="79"/>
     </row>
-    <row r="260" spans="2:54" ht="51" x14ac:dyDescent="0.2">
+    <row r="260" spans="2:55" ht="51" x14ac:dyDescent="0.2">
       <c r="B260" s="21" t="s">
         <v>208</v>
       </c>
@@ -62570,7 +62717,7 @@
       <c r="AU260" s="139"/>
       <c r="AW260" s="79"/>
     </row>
-    <row r="261" spans="2:54" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="261" spans="2:55" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B261" s="21" t="s">
         <v>209</v>
       </c>
@@ -62688,7 +62835,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="262" spans="2:54" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="262" spans="2:55" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B262" s="21" t="s">
         <v>209</v>
       </c>
@@ -62804,7 +62951,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="263" spans="2:54" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="263" spans="2:55" ht="114.75" x14ac:dyDescent="0.2">
       <c r="B263" s="21" t="s">
         <v>206</v>
       </c>
@@ -62957,7 +63104,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="264" spans="2:54" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="264" spans="2:55" ht="89.25" x14ac:dyDescent="0.2">
       <c r="B264" s="21" t="s">
         <v>207</v>
       </c>
@@ -63084,7 +63231,7 @@
       <c r="AU264" s="139"/>
       <c r="AW264" s="79"/>
     </row>
-    <row r="265" spans="2:54" ht="202.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="265" spans="2:55" ht="202.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B265" s="21" t="s">
         <v>207</v>
       </c>
@@ -63237,7 +63384,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="266" spans="2:54" s="105" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="266" spans="2:55" s="105" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
       <c r="B266" s="95" t="s">
         <v>207</v>
       </c>
@@ -63377,8 +63524,9 @@
       <c r="BB266" s="67" t="s">
         <v>324</v>
       </c>
+      <c r="BC266" s="286"/>
     </row>
-    <row r="267" spans="2:54" s="105" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="267" spans="2:55" s="105" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
       <c r="B267" s="95" t="s">
         <v>207</v>
       </c>
@@ -63520,8 +63668,9 @@
       <c r="BB267" s="67" t="s">
         <v>976</v>
       </c>
+      <c r="BC267" s="286"/>
     </row>
-    <row r="268" spans="2:54" s="105" customFormat="1" ht="90" x14ac:dyDescent="0.2">
+    <row r="268" spans="2:55" s="105" customFormat="1" ht="90" x14ac:dyDescent="0.2">
       <c r="B268" s="95" t="s">
         <v>207</v>
       </c>
@@ -63663,8 +63812,9 @@
       <c r="BB268" s="67" t="s">
         <v>976</v>
       </c>
+      <c r="BC268" s="286"/>
     </row>
-    <row r="269" spans="2:54" s="105" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="269" spans="2:55" s="105" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
       <c r="B269" s="95" t="s">
         <v>207</v>
       </c>
@@ -63806,8 +63956,9 @@
       <c r="BB269" s="67" t="s">
         <v>976</v>
       </c>
+      <c r="BC269" s="286"/>
     </row>
-    <row r="270" spans="2:54" s="105" customFormat="1" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="270" spans="2:55" s="105" customFormat="1" ht="127.5" x14ac:dyDescent="0.2">
       <c r="B270" s="95" t="s">
         <v>207</v>
       </c>
@@ -63889,8 +64040,9 @@
       <c r="AZ270" s="66"/>
       <c r="BA270" s="66"/>
       <c r="BB270" s="66"/>
+      <c r="BC270" s="286"/>
     </row>
-    <row r="271" spans="2:54" s="105" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+    <row r="271" spans="2:55" s="105" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="B271" s="95" t="s">
         <v>207</v>
       </c>
@@ -63972,8 +64124,9 @@
       <c r="AZ271" s="66"/>
       <c r="BA271" s="66"/>
       <c r="BB271" s="66"/>
+      <c r="BC271" s="286"/>
     </row>
-    <row r="272" spans="2:54" s="105" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+    <row r="272" spans="2:55" s="105" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="B272" s="95" t="s">
         <v>207</v>
       </c>
@@ -64055,8 +64208,9 @@
       <c r="AZ272" s="66"/>
       <c r="BA272" s="66"/>
       <c r="BB272" s="66"/>
+      <c r="BC272" s="286"/>
     </row>
-    <row r="273" spans="2:54" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="273" spans="2:55" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B273" s="21" t="s">
         <v>207</v>
       </c>
@@ -64191,7 +64345,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="274" spans="2:54" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="274" spans="2:55" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B274" s="21" t="s">
         <v>207</v>
       </c>
@@ -64326,7 +64480,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="275" spans="2:54" s="105" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="275" spans="2:55" s="105" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
       <c r="B275" s="95" t="s">
         <v>206</v>
       </c>
@@ -64472,8 +64626,9 @@
       <c r="AZ275" s="66"/>
       <c r="BA275" s="66"/>
       <c r="BB275" s="67"/>
+      <c r="BC275" s="286"/>
     </row>
-    <row r="276" spans="2:54" s="105" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="276" spans="2:55" s="105" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B276" s="95" t="s">
         <v>207</v>
       </c>
@@ -64619,8 +64774,9 @@
       <c r="AZ276" s="66"/>
       <c r="BA276" s="66"/>
       <c r="BB276" s="67"/>
+      <c r="BC276" s="286"/>
     </row>
-    <row r="277" spans="2:54" s="116" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="277" spans="2:55" s="116" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B277" s="106" t="s">
         <v>207</v>
       </c>
@@ -64760,8 +64916,9 @@
       <c r="AZ277" s="89"/>
       <c r="BA277" s="89"/>
       <c r="BB277" s="90"/>
+      <c r="BC277" s="286"/>
     </row>
-    <row r="278" spans="2:54" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="278" spans="2:55" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B278" s="21" t="s">
         <v>207</v>
       </c>
@@ -64860,7 +65017,7 @@
       </c>
       <c r="AW278" s="79"/>
     </row>
-    <row r="279" spans="2:54" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="279" spans="2:55" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B279" s="21" t="s">
         <v>207</v>
       </c>
@@ -65010,7 +65167,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="280" spans="2:54" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="280" spans="2:55" ht="89.25" x14ac:dyDescent="0.2">
       <c r="B280" s="21" t="s">
         <v>207</v>
       </c>
@@ -65081,7 +65238,7 @@
       </c>
       <c r="AW280" s="79"/>
     </row>
-    <row r="281" spans="2:54" x14ac:dyDescent="0.2">
+    <row r="281" spans="2:55" x14ac:dyDescent="0.2">
       <c r="B281" s="21" t="s">
         <v>207</v>
       </c>
@@ -65222,7 +65379,7 @@
       </c>
       <c r="AW281" s="79"/>
     </row>
-    <row r="282" spans="2:54" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="282" spans="2:55" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B282" s="21" t="s">
         <v>206</v>
       </c>
@@ -65364,7 +65521,7 @@
       <c r="AW282" s="79"/>
       <c r="AY282" s="92"/>
     </row>
-    <row r="283" spans="2:54" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="283" spans="2:55" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B283" s="21" t="s">
         <v>207</v>
       </c>
@@ -65505,7 +65662,7 @@
       </c>
       <c r="AW283" s="79"/>
     </row>
-    <row r="284" spans="2:54" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="284" spans="2:55" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B284" s="21" t="s">
         <v>207</v>
       </c>
@@ -65646,7 +65803,7 @@
       </c>
       <c r="AW284" s="79"/>
     </row>
-    <row r="285" spans="2:54" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="285" spans="2:55" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B285" s="21" t="s">
         <v>207</v>
       </c>
@@ -65787,7 +65944,7 @@
       </c>
       <c r="AW285" s="79"/>
     </row>
-    <row r="286" spans="2:54" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="286" spans="2:55" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B286" s="21" t="s">
         <v>207</v>
       </c>
@@ -65928,7 +66085,7 @@
       </c>
       <c r="AW286" s="79"/>
     </row>
-    <row r="287" spans="2:54" ht="51" x14ac:dyDescent="0.2">
+    <row r="287" spans="2:55" ht="51" x14ac:dyDescent="0.2">
       <c r="B287" s="21" t="s">
         <v>206</v>
       </c>
@@ -66066,7 +66223,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="288" spans="2:54" ht="51" x14ac:dyDescent="0.2">
+    <row r="288" spans="2:55" ht="51" x14ac:dyDescent="0.2">
       <c r="B288" s="21" t="s">
         <v>207</v>
       </c>
@@ -66135,7 +66292,7 @@
       </c>
       <c r="AW288" s="79"/>
     </row>
-    <row r="289" spans="2:54" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="289" spans="2:55" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B289" s="21" t="s">
         <v>207</v>
       </c>
@@ -66268,7 +66425,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="290" spans="2:54" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="290" spans="2:55" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B290" s="21" t="s">
         <v>207</v>
       </c>
@@ -66403,7 +66560,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="291" spans="2:54" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="291" spans="2:55" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B291" s="21" t="s">
         <v>207</v>
       </c>
@@ -66538,7 +66695,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="292" spans="2:54" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="292" spans="2:55" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B292" s="21" t="s">
         <v>206</v>
       </c>
@@ -66601,7 +66758,7 @@
       </c>
       <c r="AW292" s="79"/>
     </row>
-    <row r="293" spans="2:54" ht="51" x14ac:dyDescent="0.2">
+    <row r="293" spans="2:55" ht="51" x14ac:dyDescent="0.2">
       <c r="B293" s="21" t="s">
         <v>207</v>
       </c>
@@ -66664,7 +66821,7 @@
       </c>
       <c r="AW293" s="79"/>
     </row>
-    <row r="294" spans="2:54" s="105" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="294" spans="2:55" s="105" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="B294" s="95" t="s">
         <v>207</v>
       </c>
@@ -66732,8 +66889,9 @@
       <c r="AZ294" s="66"/>
       <c r="BA294" s="66"/>
       <c r="BB294" s="66"/>
+      <c r="BC294" s="286"/>
     </row>
-    <row r="295" spans="2:54" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="295" spans="2:55" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B295" s="21" t="s">
         <v>207</v>
       </c>
@@ -66796,7 +66954,7 @@
       </c>
       <c r="AW295" s="79"/>
     </row>
-    <row r="296" spans="2:54" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="296" spans="2:55" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B296" s="21" t="s">
         <v>207</v>
       </c>
@@ -66859,7 +67017,7 @@
       </c>
       <c r="AW296" s="79"/>
     </row>
-    <row r="297" spans="2:54" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="297" spans="2:55" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B297" s="21" t="s">
         <v>207</v>
       </c>
@@ -66922,7 +67080,7 @@
       </c>
       <c r="AW297" s="79"/>
     </row>
-    <row r="298" spans="2:54" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="298" spans="2:55" ht="114.75" x14ac:dyDescent="0.2">
       <c r="B298" s="21" t="s">
         <v>207</v>
       </c>
@@ -66993,7 +67151,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="299" spans="2:54" s="105" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="2:55" s="105" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B299" s="117" t="s">
         <v>207</v>
       </c>
@@ -67061,8 +67219,9 @@
       <c r="AZ299" s="66"/>
       <c r="BA299" s="66"/>
       <c r="BB299" s="66"/>
+      <c r="BC299" s="286"/>
     </row>
-    <row r="300" spans="2:54" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="300" spans="2:55" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <autoFilter ref="B1:BB302">
     <filterColumn colId="6" showButton="0"/>
@@ -67138,155 +67297,155 @@
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="B1:AU1 B6:AU19 B2:AT5 B21:AU40 B20:AT20 B60:AU66 B59:AT59 B92:AU95 B91:AT91 B125:AU134 B124:AT124 B136:AU138 B135:AT135 B195:AU195 B198:AU198 B228:AU301 B200:AU202 B199:AT199 B204:AU205 B203:AT203 B207:AU210 B206:AT206 B216:AU218 B213:AT215 B221:AU221 B219:AT220 B224:AU224 B222:AT223 B225:AT227 B44:AU45 B43:AT43 B53:AU58 B52:AT52 B173:AU173 B175:AU175 B174:AT174 B212:AU212 B211:AT211 B140:AU141 B139:AT139 B178:AU187 B171:AT172 B145:AU146 B143:AT144 B148:AU170 B147:AT147 B176:AT177 B48:AU51 B46:AT47 B68:AU76 B67:AT67 B77:AT77 B85:AU90 B84:AT84 B97:AU98 B96:AT96 B109:AT109 B196:AT197 B188:AT194 B78:AU83 B42:AU42 B100:AU108 B110:AU123">
-    <cfRule type="expression" dxfId="40" priority="90" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="90" stopIfTrue="1">
       <formula>LEFT($C1,2)="BG"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:AU19 H21:AU40 H20:AT20 H60:AU66 H59:AT59 H92:AU95 H91:AT91 H125:AU134 H124:AT124 H136:AU138 H135:AT135 H195:AU195 H198:AU198 H228:AU301 H200:AU202 H199:AT199 H204:AU205 H203:AT203 H207:AU210 H206:AT206 H216:AU218 H213:AT215 H221:AU221 H219:AT220 H224:AU224 H222:AT223 H225:AT227 H44:AU45 H43:AT43 H53:AU58 H52:AT52 H173:AU173 H175:AU175 H174:AT174 H212:AU212 H211:AT211 H140:AU141 H139:AT139 H178:AU187 H171:AT172 H145:AU146 H143:AT144 H148:AU170 H147:AT147 H176:AT177 H48:AU51 H46:AT47 H68:AU76 H67:AT67 H78:AU83 H77:AT77 H85:AU90 H84:AT84 H97:AU98 H96:AT96 H109:AT109 H196:AT197 H188:AT194 H42:AU42 H100:AU108 H110:AU123">
-    <cfRule type="cellIs" dxfId="39" priority="91" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="91" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="92" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="92" operator="equal">
       <formula>"CM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="93" operator="equal">
       <formula>"M"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AW24:BB24">
-    <cfRule type="expression" dxfId="36" priority="86" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="86" stopIfTrue="1">
       <formula>LEFT($C24,2)="BG"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AW24:BB24">
-    <cfRule type="cellIs" dxfId="35" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="87" operator="equal">
       <formula>"CM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="88" operator="equal">
       <formula>"M"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="89" operator="equal">
       <formula>"O"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU20">
-    <cfRule type="expression" dxfId="32" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="29" stopIfTrue="1">
       <formula>LEFT($C20,2)="BG"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU59">
-    <cfRule type="expression" dxfId="31" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="28" stopIfTrue="1">
       <formula>LEFT($C59,2)="BG"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU91">
-    <cfRule type="expression" dxfId="30" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="27" stopIfTrue="1">
       <formula>LEFT($C91,2)="BG"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU124">
-    <cfRule type="expression" dxfId="29" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="26" stopIfTrue="1">
       <formula>LEFT($C124,2)="BG"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU135">
-    <cfRule type="expression" dxfId="28" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="25" stopIfTrue="1">
       <formula>LEFT($C135,2)="BG"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU43">
-    <cfRule type="expression" dxfId="27" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="21" stopIfTrue="1">
       <formula>LEFT($C43,2)="BG"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU43">
-    <cfRule type="cellIs" dxfId="26" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="22" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="23" operator="equal">
       <formula>"CM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="24" operator="equal">
       <formula>"M"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU52">
-    <cfRule type="expression" dxfId="23" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="17" stopIfTrue="1">
       <formula>LEFT($C52,2)="BG"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU52">
-    <cfRule type="cellIs" dxfId="22" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
       <formula>"CM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="20" operator="equal">
       <formula>"M"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU197">
-    <cfRule type="expression" dxfId="19" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="13" stopIfTrue="1">
       <formula>LEFT($C197,2)="BG"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU197">
-    <cfRule type="cellIs" dxfId="18" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
       <formula>"CM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
       <formula>"M"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B41:AU41">
-    <cfRule type="expression" dxfId="15" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="9" stopIfTrue="1">
       <formula>LEFT($C41,2)="BG"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H41:AU41">
-    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
       <formula>"CM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
       <formula>"M"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B99:AU99">
-    <cfRule type="expression" dxfId="11" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="5" stopIfTrue="1">
       <formula>LEFT($C99,2)="BG"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H99:AU99">
-    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>"CM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
       <formula>"M"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B142:AU142">
-    <cfRule type="expression" dxfId="7" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="1" stopIfTrue="1">
       <formula>LEFT($C142,2)="BG"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H142:AU142">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"O"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"CM"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"M"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -67306,23 +67465,23 @@
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="37.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="140.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="281" t="s">
+      <c r="A1" s="283" t="s">
         <v>683</v>
       </c>
-      <c r="B1" s="282"/>
+      <c r="B1" s="284"/>
     </row>
     <row r="2" spans="1:2" ht="50.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="283" t="s">
+      <c r="A2" s="285" t="s">
         <v>969</v>
       </c>
-      <c r="B2" s="283"/>
+      <c r="B2" s="285"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="57"/>
@@ -67365,16 +67524,16 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="277" t="s">
+      <c r="A9" s="279" t="s">
         <v>415</v>
       </c>
-      <c r="B9" s="279" t="s">
+      <c r="B9" s="281" t="s">
         <v>393</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="278"/>
-      <c r="B10" s="280"/>
+      <c r="A10" s="280"/>
+      <c r="B10" s="282"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="10"/>
@@ -67649,7 +67808,7 @@
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="105"/>
@@ -67694,7 +67853,7 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
Lastest version of the ePO Ontology after the WGM (17th and 19th September)
</commit_message>
<xml_diff>
--- a/v2.0.1/Ontology_eForms_Mapping.xlsx
+++ b/v2.0.1/Ontology_eForms_Mapping.xlsx
@@ -407,7 +407,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12377" uniqueCount="1604">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12393" uniqueCount="1617">
   <si>
     <t>ID</t>
   </si>
@@ -7849,6 +7849,77 @@
     <t>Procedure has Lot,
 Lot applied SubmissionTerms,
 SubmissionTerms haseSubmissionCommunication</t>
+  </si>
+  <si>
+    <t>Procedure has Lot,
+Lot has AwardCriterion,
+AwardCriterion hasFormula which is inherited from Criterion</t>
+  </si>
+  <si>
+    <t>Procedure.Lot.AwardCriterion.Formula</t>
+  </si>
+  <si>
+    <t>The expression used to find a result.
+Additional information: 
+This expression is usually a mathematical formula, but it can be an informal description of the way in which the result will be calculated.
+WG Approval 19/09/2019</t>
+  </si>
+  <si>
+    <t>Procedure.Lot.AwardCriterion.WeightingJustification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explanation about why the actual weighting model is chosen. 
+Additional information: 
+In eNotification: This property is specifically used to describe why the order of importance is used over another weighting model.
+In ESPD: This is used to explain other complex models of weighting for transparency reasons. 
+WG Approval 19/09/2019 </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Procedure has Lot,
+Lot has AwardCriterion,
+AwardCriterion hasWeightingJustification which is inherited from Criterion
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>See recital 90 Directive 24</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Methods used for conducting procurement procedure.
+Addtional information:
+Several techniques can be combined in one single procurement procedure (e.g. eAuction can be carried out in a Framework Agreement or DPS).
+WG Approval 19/09/2019 </t>
+  </si>
+  <si>
+    <t>Procedure has Lot,
+Lot uses Techniques,
+Lot hasID Identifier</t>
+  </si>
+  <si>
+    <t>Procedure.Lot.ID,
+Lot.Techniques</t>
+  </si>
+  <si>
+    <t>Procedure.FrameworkAgreementTerms.FrameworkAgreementType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The form of framework agreement used in a procurement procedure.
+WG Approval 19/09/2019 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Procedure uses Framework Agreement Terms,
+Framework Agreement Terms hasFrameworkAgreementType Code
+</t>
+  </si>
+  <si>
+    <t>Although eForms uses the code none, the ontology does not use this code as the design approach in the ontology is base in the existance or absence of specific property and associated class (e.g. Procedure has Technique, Technique is of type of Framework Agreement. So if the class does not exist, it can not be represented).</t>
   </si>
 </sst>
 </file>
@@ -9098,7 +9169,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="288">
+  <cellXfs count="289">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -9812,6 +9883,69 @@
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -9827,21 +9961,6 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -9852,51 +9971,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -10649,10 +10723,10 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:XFD300"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A163" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A168" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="AU161" sqref="AU161"/>
+      <selection pane="bottomLeft" activeCell="C169" sqref="A169:XFD169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10697,95 +10771,95 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:55" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="274" t="s">
+      <c r="B1" s="253" t="s">
         <v>205</v>
       </c>
-      <c r="C1" s="266" t="s">
+      <c r="C1" s="256" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="266" t="s">
+      <c r="D1" s="256" t="s">
         <v>577</v>
       </c>
-      <c r="E1" s="266" t="s">
+      <c r="E1" s="256" t="s">
         <v>319</v>
       </c>
-      <c r="F1" s="266" t="s">
+      <c r="F1" s="256" t="s">
         <v>330</v>
       </c>
-      <c r="G1" s="278" t="s">
+      <c r="G1" s="263" t="s">
         <v>333</v>
       </c>
-      <c r="H1" s="257" t="s">
+      <c r="H1" s="259" t="s">
         <v>540</v>
       </c>
-      <c r="I1" s="258"/>
-      <c r="J1" s="258"/>
-      <c r="K1" s="258"/>
-      <c r="L1" s="258"/>
-      <c r="M1" s="258"/>
-      <c r="N1" s="277"/>
-      <c r="O1" s="259"/>
-      <c r="P1" s="257" t="s">
+      <c r="I1" s="260"/>
+      <c r="J1" s="260"/>
+      <c r="K1" s="260"/>
+      <c r="L1" s="260"/>
+      <c r="M1" s="260"/>
+      <c r="N1" s="261"/>
+      <c r="O1" s="262"/>
+      <c r="P1" s="259" t="s">
         <v>541</v>
       </c>
-      <c r="Q1" s="258"/>
-      <c r="R1" s="258"/>
-      <c r="S1" s="258"/>
-      <c r="T1" s="258"/>
-      <c r="U1" s="258"/>
-      <c r="V1" s="258"/>
-      <c r="W1" s="258"/>
-      <c r="X1" s="258"/>
-      <c r="Y1" s="258"/>
-      <c r="Z1" s="258"/>
-      <c r="AA1" s="258"/>
-      <c r="AB1" s="258"/>
-      <c r="AC1" s="258"/>
-      <c r="AD1" s="259"/>
-      <c r="AE1" s="257" t="s">
+      <c r="Q1" s="260"/>
+      <c r="R1" s="260"/>
+      <c r="S1" s="260"/>
+      <c r="T1" s="260"/>
+      <c r="U1" s="260"/>
+      <c r="V1" s="260"/>
+      <c r="W1" s="260"/>
+      <c r="X1" s="260"/>
+      <c r="Y1" s="260"/>
+      <c r="Z1" s="260"/>
+      <c r="AA1" s="260"/>
+      <c r="AB1" s="260"/>
+      <c r="AC1" s="260"/>
+      <c r="AD1" s="262"/>
+      <c r="AE1" s="259" t="s">
         <v>542</v>
       </c>
-      <c r="AF1" s="258"/>
-      <c r="AG1" s="258"/>
-      <c r="AH1" s="259"/>
-      <c r="AI1" s="257" t="s">
+      <c r="AF1" s="260"/>
+      <c r="AG1" s="260"/>
+      <c r="AH1" s="262"/>
+      <c r="AI1" s="259" t="s">
         <v>543</v>
       </c>
-      <c r="AJ1" s="258"/>
-      <c r="AK1" s="258"/>
-      <c r="AL1" s="258"/>
-      <c r="AM1" s="258"/>
-      <c r="AN1" s="258"/>
-      <c r="AO1" s="258"/>
-      <c r="AP1" s="258"/>
-      <c r="AQ1" s="259"/>
-      <c r="AR1" s="257" t="s">
+      <c r="AJ1" s="260"/>
+      <c r="AK1" s="260"/>
+      <c r="AL1" s="260"/>
+      <c r="AM1" s="260"/>
+      <c r="AN1" s="260"/>
+      <c r="AO1" s="260"/>
+      <c r="AP1" s="260"/>
+      <c r="AQ1" s="262"/>
+      <c r="AR1" s="259" t="s">
         <v>963</v>
       </c>
-      <c r="AS1" s="258"/>
-      <c r="AT1" s="259"/>
-      <c r="AU1" s="262" t="s">
+      <c r="AS1" s="260"/>
+      <c r="AT1" s="262"/>
+      <c r="AU1" s="278" t="s">
         <v>1158</v>
       </c>
-      <c r="AV1" s="263" t="s">
+      <c r="AV1" s="279" t="s">
         <v>1144</v>
       </c>
-      <c r="AX1" s="264" t="s">
+      <c r="AX1" s="280" t="s">
         <v>971</v>
       </c>
-      <c r="AY1" s="265"/>
-      <c r="AZ1" s="265"/>
+      <c r="AY1" s="281"/>
+      <c r="AZ1" s="281"/>
       <c r="BC1" s="250" t="s">
         <v>1546</v>
       </c>
     </row>
     <row r="2" spans="2:55" ht="14.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="275"/>
-      <c r="C2" s="267"/>
-      <c r="D2" s="267"/>
-      <c r="E2" s="267"/>
-      <c r="F2" s="267"/>
-      <c r="G2" s="279"/>
+      <c r="B2" s="254"/>
+      <c r="C2" s="257"/>
+      <c r="D2" s="257"/>
+      <c r="E2" s="257"/>
+      <c r="F2" s="257"/>
+      <c r="G2" s="264"/>
       <c r="H2" s="38">
         <v>1</v>
       </c>
@@ -10903,115 +10977,115 @@
       <c r="AT2" s="127">
         <v>39</v>
       </c>
-      <c r="AU2" s="262"/>
-      <c r="AV2" s="263"/>
+      <c r="AU2" s="278"/>
+      <c r="AV2" s="279"/>
       <c r="AW2" s="130"/>
-      <c r="AX2" s="252" t="s">
+      <c r="AX2" s="273" t="s">
         <v>972</v>
       </c>
-      <c r="AY2" s="252" t="s">
+      <c r="AY2" s="273" t="s">
         <v>973</v>
       </c>
-      <c r="AZ2" s="252" t="s">
+      <c r="AZ2" s="273" t="s">
         <v>974</v>
       </c>
       <c r="BA2" s="59"/>
-      <c r="BB2" s="252" t="s">
+      <c r="BB2" s="273" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="3" spans="2:55" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="275"/>
-      <c r="C3" s="267"/>
-      <c r="D3" s="267"/>
-      <c r="E3" s="267"/>
-      <c r="F3" s="267"/>
-      <c r="G3" s="279"/>
-      <c r="H3" s="270" t="s">
+      <c r="B3" s="254"/>
+      <c r="C3" s="257"/>
+      <c r="D3" s="257"/>
+      <c r="E3" s="257"/>
+      <c r="F3" s="257"/>
+      <c r="G3" s="264"/>
+      <c r="H3" s="268" t="s">
         <v>373</v>
       </c>
-      <c r="I3" s="261"/>
-      <c r="J3" s="273"/>
-      <c r="K3" s="272" t="s">
+      <c r="I3" s="269"/>
+      <c r="J3" s="272"/>
+      <c r="K3" s="271" t="s">
         <v>374</v>
       </c>
-      <c r="L3" s="261"/>
-      <c r="M3" s="273"/>
-      <c r="N3" s="272" t="s">
+      <c r="L3" s="269"/>
+      <c r="M3" s="272"/>
+      <c r="N3" s="271" t="s">
         <v>375</v>
       </c>
-      <c r="O3" s="269"/>
-      <c r="P3" s="270" t="s">
+      <c r="O3" s="267"/>
+      <c r="P3" s="268" t="s">
         <v>376</v>
       </c>
-      <c r="Q3" s="273"/>
-      <c r="R3" s="272" t="s">
+      <c r="Q3" s="272"/>
+      <c r="R3" s="271" t="s">
         <v>377</v>
       </c>
-      <c r="S3" s="261"/>
-      <c r="T3" s="273"/>
+      <c r="S3" s="269"/>
+      <c r="T3" s="272"/>
       <c r="U3" s="37" t="s">
         <v>562</v>
       </c>
-      <c r="V3" s="272" t="s">
+      <c r="V3" s="271" t="s">
         <v>378</v>
       </c>
-      <c r="W3" s="261"/>
-      <c r="X3" s="261"/>
-      <c r="Y3" s="273"/>
-      <c r="Z3" s="272" t="s">
+      <c r="W3" s="269"/>
+      <c r="X3" s="269"/>
+      <c r="Y3" s="272"/>
+      <c r="Z3" s="271" t="s">
         <v>379</v>
       </c>
-      <c r="AA3" s="273"/>
+      <c r="AA3" s="272"/>
       <c r="AB3" s="37" t="s">
         <v>680</v>
       </c>
-      <c r="AC3" s="272" t="s">
+      <c r="AC3" s="271" t="s">
         <v>681</v>
       </c>
-      <c r="AD3" s="269"/>
-      <c r="AE3" s="270" t="s">
+      <c r="AD3" s="267"/>
+      <c r="AE3" s="268" t="s">
         <v>682</v>
       </c>
-      <c r="AF3" s="261"/>
-      <c r="AG3" s="261"/>
-      <c r="AH3" s="269"/>
-      <c r="AI3" s="270" t="s">
+      <c r="AF3" s="269"/>
+      <c r="AG3" s="269"/>
+      <c r="AH3" s="267"/>
+      <c r="AI3" s="268" t="s">
         <v>382</v>
       </c>
-      <c r="AJ3" s="261"/>
-      <c r="AK3" s="261"/>
-      <c r="AL3" s="271"/>
-      <c r="AM3" s="260" t="s">
+      <c r="AJ3" s="269"/>
+      <c r="AK3" s="269"/>
+      <c r="AL3" s="270"/>
+      <c r="AM3" s="266" t="s">
         <v>383</v>
       </c>
-      <c r="AN3" s="261"/>
-      <c r="AO3" s="271"/>
-      <c r="AP3" s="260" t="s">
+      <c r="AN3" s="269"/>
+      <c r="AO3" s="270"/>
+      <c r="AP3" s="266" t="s">
         <v>681</v>
       </c>
-      <c r="AQ3" s="269"/>
-      <c r="AR3" s="260" t="s">
+      <c r="AQ3" s="267"/>
+      <c r="AR3" s="266" t="s">
         <v>963</v>
       </c>
-      <c r="AS3" s="261"/>
-      <c r="AT3" s="261"/>
-      <c r="AU3" s="262"/>
-      <c r="AV3" s="263"/>
+      <c r="AS3" s="269"/>
+      <c r="AT3" s="269"/>
+      <c r="AU3" s="278"/>
+      <c r="AV3" s="279"/>
       <c r="AW3" s="131"/>
-      <c r="AX3" s="253"/>
-      <c r="AY3" s="253"/>
-      <c r="AZ3" s="253"/>
+      <c r="AX3" s="274"/>
+      <c r="AY3" s="274"/>
+      <c r="AZ3" s="274"/>
       <c r="BA3" s="60"/>
-      <c r="BB3" s="253"/>
+      <c r="BB3" s="274"/>
     </row>
     <row r="4" spans="2:55" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="276"/>
-      <c r="C4" s="268"/>
-      <c r="D4" s="268"/>
-      <c r="E4" s="268"/>
-      <c r="F4" s="268"/>
-      <c r="G4" s="280"/>
+      <c r="B4" s="255"/>
+      <c r="C4" s="258"/>
+      <c r="D4" s="258"/>
+      <c r="E4" s="258"/>
+      <c r="F4" s="258"/>
+      <c r="G4" s="265"/>
       <c r="H4" s="28" t="s">
         <v>386</v>
       </c>
@@ -11129,16 +11203,16 @@
       <c r="AT4" s="31" t="s">
         <v>389</v>
       </c>
-      <c r="AU4" s="262"/>
-      <c r="AV4" s="263"/>
+      <c r="AU4" s="278"/>
+      <c r="AV4" s="279"/>
       <c r="AW4" s="212" t="s">
         <v>1302</v>
       </c>
-      <c r="AX4" s="253"/>
-      <c r="AY4" s="253"/>
-      <c r="AZ4" s="253"/>
+      <c r="AX4" s="274"/>
+      <c r="AY4" s="274"/>
+      <c r="AZ4" s="274"/>
       <c r="BA4" s="60"/>
-      <c r="BB4" s="253"/>
+      <c r="BB4" s="274"/>
     </row>
     <row r="5" spans="2:55" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="201"/>
@@ -11188,11 +11262,11 @@
       <c r="AT5" s="208"/>
       <c r="AU5" s="204"/>
       <c r="AV5" s="213"/>
-      <c r="AW5" s="254" t="s">
+      <c r="AW5" s="275" t="s">
         <v>1299</v>
       </c>
-      <c r="AX5" s="255"/>
-      <c r="AY5" s="256"/>
+      <c r="AX5" s="276"/>
+      <c r="AY5" s="277"/>
       <c r="AZ5" s="131"/>
       <c r="BA5" s="205"/>
       <c r="BB5" s="205"/>
@@ -50137,7 +50211,7 @@
         <v>1540</v>
       </c>
     </row>
-    <row r="164" spans="2:55" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="164" spans="2:55" ht="127.5" x14ac:dyDescent="0.2">
       <c r="B164" s="21" t="s">
         <v>207</v>
       </c>
@@ -50268,12 +50342,23 @@
       <c r="AS164" s="23"/>
       <c r="AT164" s="24"/>
       <c r="AU164" s="139"/>
-      <c r="AW164" s="79"/>
+      <c r="AV164" s="167">
+        <v>20190919</v>
+      </c>
+      <c r="AW164" s="79" t="s">
+        <v>1604</v>
+      </c>
+      <c r="AX164" s="80" t="s">
+        <v>1605</v>
+      </c>
+      <c r="AY164" s="80" t="s">
+        <v>1606</v>
+      </c>
       <c r="BC164" s="250" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="165" spans="2:55" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="165" spans="2:55" ht="140.25" x14ac:dyDescent="0.2">
       <c r="B165" s="21" t="s">
         <v>207</v>
       </c>
@@ -50392,7 +50477,21 @@
       <c r="AS165" s="23"/>
       <c r="AT165" s="24"/>
       <c r="AU165" s="139"/>
-      <c r="AW165" s="79"/>
+      <c r="AV165" s="167">
+        <v>20190919</v>
+      </c>
+      <c r="AW165" s="63" t="s">
+        <v>1609</v>
+      </c>
+      <c r="AX165" s="80" t="s">
+        <v>1607</v>
+      </c>
+      <c r="AY165" s="80" t="s">
+        <v>1608</v>
+      </c>
+      <c r="BB165" s="58" t="s">
+        <v>324</v>
+      </c>
       <c r="BC165" s="250" t="s">
         <v>323</v>
       </c>
@@ -50534,7 +50633,13 @@
         <v>369</v>
       </c>
       <c r="AU166" s="139"/>
+      <c r="AV166" s="138">
+        <v>20190919</v>
+      </c>
       <c r="AW166" s="79"/>
+      <c r="AY166" s="62" t="s">
+        <v>1610</v>
+      </c>
       <c r="BC166" s="250" t="s">
         <v>1541</v>
       </c>
@@ -50674,7 +50779,18 @@
         <v>369</v>
       </c>
       <c r="AU167" s="139"/>
-      <c r="AW167" s="79"/>
+      <c r="AV167" s="138">
+        <v>20190919</v>
+      </c>
+      <c r="AW167" s="63" t="s">
+        <v>1611</v>
+      </c>
+      <c r="AX167" s="62" t="s">
+        <v>1612</v>
+      </c>
+      <c r="BB167" s="252" t="s">
+        <v>320</v>
+      </c>
       <c r="BC167" s="250" t="s">
         <v>1542</v>
       </c>
@@ -50805,17 +50921,27 @@
       <c r="AT168" s="101" t="s">
         <v>369</v>
       </c>
-      <c r="AU168" s="139"/>
-      <c r="AV168" s="70">
-        <v>20190305</v>
-      </c>
-      <c r="AW168" s="69"/>
-      <c r="AX168" s="70"/>
-      <c r="AY168" s="70"/>
+      <c r="AU168" s="139" t="s">
+        <v>1616</v>
+      </c>
+      <c r="AV168" s="167">
+        <v>20190919</v>
+      </c>
+      <c r="AW168" s="64" t="s">
+        <v>1615</v>
+      </c>
+      <c r="AX168" s="65" t="s">
+        <v>1613</v>
+      </c>
+      <c r="AY168" s="65" t="s">
+        <v>1614</v>
+      </c>
       <c r="AZ168" s="66"/>
       <c r="BA168" s="66"/>
-      <c r="BB168" s="66"/>
-      <c r="BC168" s="250" t="s">
+      <c r="BB168" s="67" t="s">
+        <v>321</v>
+      </c>
+      <c r="BC168" s="251" t="s">
         <v>1543</v>
       </c>
     </row>
@@ -67674,13 +67800,17 @@
     <filterColumn colId="49" showButton="0"/>
   </autoFilter>
   <mergeCells count="32">
-    <mergeCell ref="B1:B4"/>
-    <mergeCell ref="D1:D4"/>
-    <mergeCell ref="E1:E4"/>
-    <mergeCell ref="H1:O1"/>
-    <mergeCell ref="P1:AD1"/>
-    <mergeCell ref="F1:F4"/>
-    <mergeCell ref="G1:G4"/>
+    <mergeCell ref="BB2:BB4"/>
+    <mergeCell ref="AW5:AY5"/>
+    <mergeCell ref="AR1:AT1"/>
+    <mergeCell ref="AR3:AT3"/>
+    <mergeCell ref="AI1:AQ1"/>
+    <mergeCell ref="AU1:AU4"/>
+    <mergeCell ref="AV1:AV4"/>
+    <mergeCell ref="AX1:AZ1"/>
+    <mergeCell ref="AX2:AX4"/>
+    <mergeCell ref="AY2:AY4"/>
+    <mergeCell ref="AZ2:AZ4"/>
     <mergeCell ref="AE1:AH1"/>
     <mergeCell ref="C1:C4"/>
     <mergeCell ref="AP3:AQ3"/>
@@ -67695,17 +67825,13 @@
     <mergeCell ref="K3:M3"/>
     <mergeCell ref="N3:O3"/>
     <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="BB2:BB4"/>
-    <mergeCell ref="AW5:AY5"/>
-    <mergeCell ref="AR1:AT1"/>
-    <mergeCell ref="AR3:AT3"/>
-    <mergeCell ref="AI1:AQ1"/>
-    <mergeCell ref="AU1:AU4"/>
-    <mergeCell ref="AV1:AV4"/>
-    <mergeCell ref="AX1:AZ1"/>
-    <mergeCell ref="AX2:AX4"/>
-    <mergeCell ref="AY2:AY4"/>
-    <mergeCell ref="AZ2:AZ4"/>
+    <mergeCell ref="B1:B4"/>
+    <mergeCell ref="D1:D4"/>
+    <mergeCell ref="E1:E4"/>
+    <mergeCell ref="H1:O1"/>
+    <mergeCell ref="P1:AD1"/>
+    <mergeCell ref="F1:F4"/>
+    <mergeCell ref="G1:G4"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="B1:AU1 B6:AU19 B2:AT5 B21:AU40 B20:AT20 B60:AU66 B59:AT59 B92:AU95 B91:AT91 B125:AU134 B124:AT124 B136:AU138 B135:AT135 B195:AU195 B198:AU198 B228:AU301 B200:AU202 B199:AT199 B204:AU205 B203:AT203 B207:AU210 B206:AT206 B216:AU218 B213:AT215 B221:AU221 B219:AT220 B224:AU224 B222:AT223 B225:AT227 B44:AU45 B43:AT43 B53:AU58 B52:AT52 B173:AU173 B175:AU175 B174:AT174 B212:AU212 B211:AT211 B140:AU141 B139:AT139 B178:AU187 B171:AT172 B145:AU146 B143:AT144 B148:AU170 B147:AT147 B176:AT177 B48:AU51 B46:AT47 B68:AU76 B67:AT67 B77:AT77 B85:AU90 B84:AT84 B97:AU98 B96:AT96 B109:AT109 B196:AT197 B188:AT194 B78:AU83 B42:AU42 B100:AU108 B110:AU123">
@@ -67884,16 +68010,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="285" t="s">
+      <c r="A1" s="286" t="s">
         <v>683</v>
       </c>
-      <c r="B1" s="286"/>
+      <c r="B1" s="287"/>
     </row>
     <row r="2" spans="1:2" ht="50.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="287" t="s">
+      <c r="A2" s="288" t="s">
         <v>969</v>
       </c>
-      <c r="B2" s="287"/>
+      <c r="B2" s="288"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="57"/>
@@ -67936,16 +68062,16 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="281" t="s">
+      <c r="A9" s="282" t="s">
         <v>415</v>
       </c>
-      <c r="B9" s="283" t="s">
+      <c r="B9" s="284" t="s">
         <v>393</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="282"/>
-      <c r="B10" s="284"/>
+      <c r="A10" s="283"/>
+      <c r="B10" s="285"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="10"/>
@@ -68450,22 +68576,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <AresNumber xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </AresNumber>
-    <Unit_Dir0_tax xmlns="http://schemas.microsoft.com/sharepoint/v3/fields">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </Unit_Dir0_tax>
-    <TaxCatchAll xmlns="f35f5637-fabd-4565-b1d5-90ce7b582d39"/>
-    <Document_x0020_Description xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="OP Document" ma:contentTypeID="0x010100AAE994419BC24CED8BF9A98B0A371F990017A88DF331AD644593F8539DE8063C57" ma:contentTypeVersion="62" ma:contentTypeDescription="Create in this document library a blank document" ma:contentTypeScope="" ma:versionID="3593b262fa03f1d9b866c55d4b8338ad">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns3="f35f5637-fabd-4565-b1d5-90ce7b582d39" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="419bf95d33474cc0abbef48644714d41" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -68648,9 +68758,29 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <AresNumber xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </AresNumber>
+    <Unit_Dir0_tax xmlns="http://schemas.microsoft.com/sharepoint/v3/fields">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </Unit_Dir0_tax>
+    <TaxCatchAll xmlns="f35f5637-fabd-4565-b1d5-90ce7b582d39"/>
+    <Document_x0020_Description xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="c2ecfd70-f0a7-4227-9d3f-c0584232298e" ContentTypeId="0x010100AAE994419BC24CED8BF9A98B0A371F99" PreviousValue="false"/>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -68665,32 +68795,10 @@
 
 <file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="c2ecfd70-f0a7-4227-9d3f-c0584232298e" ContentTypeId="0x010100AAE994419BC24CED8BF9A98B0A371F99" PreviousValue="false"/>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C5668C2-9E4E-41FF-A600-007B45A14DC5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="f35f5637-fabd-4565-b1d5-90ce7b582d39"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C5654C0-3855-420F-8C22-DF4B544C7F47}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -68710,10 +68818,28 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C5668C2-9E4E-41FF-A600-007B45A14DC5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="f35f5637-fabd-4565-b1d5-90ce7b582d39"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91444F0C-2F56-43B8-A080-17A1842BA733}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB384150-4BBF-4CDD-8953-A011DFA23524}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -68727,9 +68853,9 @@
 </file>
 
 <file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB384150-4BBF-4CDD-8953-A011DFA23524}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91444F0C-2F56-43B8-A080-17A1842BA733}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>